<commit_message>
Update ORM Statistics Official Result.xlsx
</commit_message>
<xml_diff>
--- a/assets/ORM Statistics Official Result.xlsx
+++ b/assets/ORM Statistics Official Result.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dongenergy-my.sharepoint.com/personal/mipen_orsted_dk/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MichaelP\Source\Repos\GitHub\RepoDb.NET\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C970996-3557-4966-A55C-F641DBFA3075}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-7440" windowWidth="38616" windowHeight="21360" tabRatio="538" xr2:uid="{2E957980-B71D-4FA2-92D5-8C2A268BA509}"/>
+    <workbookView xWindow="22932" yWindow="-7440" windowWidth="38616" windowHeight="21360" tabRatio="538"/>
   </bookViews>
   <sheets>
     <sheet name="Entries" sheetId="1" r:id="rId1"/>
@@ -165,7 +164,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -222,7 +221,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -275,6 +274,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -402,8 +402,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -445,7 +446,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -542,8 +543,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -585,7 +587,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -682,8 +684,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -725,7 +728,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -822,8 +825,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -865,7 +869,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -962,8 +966,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1005,7 +1010,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -1102,8 +1107,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1145,7 +1151,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -1245,8 +1251,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1288,7 +1295,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -1388,8 +1395,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1431,7 +1439,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000007-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -1531,8 +1539,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1574,7 +1583,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000008-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -1674,8 +1683,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1717,7 +1727,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000009-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -1817,8 +1827,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1860,7 +1871,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000A-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -1960,8 +1971,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2003,7 +2015,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000B-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -2106,8 +2118,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2149,7 +2162,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000C-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -2252,8 +2265,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2295,7 +2309,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000D-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -2398,8 +2412,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2441,7 +2456,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000E-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -2544,8 +2559,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2587,7 +2603,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000F-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -2690,8 +2706,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2733,7 +2750,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000010-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -2836,8 +2853,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2879,7 +2897,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000011-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -2979,8 +2997,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3022,7 +3041,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000012-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -3039,11 +3058,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="1789779311"/>
-        <c:axId val="1794294607"/>
+        <c:axId val="-1250758240"/>
+        <c:axId val="-1250752800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1789779311"/>
+        <c:axId val="-1250758240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3086,7 +3105,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1794294607"/>
+        <c:crossAx val="-1250752800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3094,7 +3113,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1794294607"/>
+        <c:axId val="-1250752800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3145,7 +3164,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1789779311"/>
+        <c:crossAx val="-1250758240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3236,7 +3255,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3275,6 +3294,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3468,7 +3488,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8BAC-48B0-8D94-A3CB19B3312A}"/>
             </c:ext>
@@ -3631,7 +3651,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-8BAC-48B0-8D94-A3CB19B3312A}"/>
             </c:ext>
@@ -3647,11 +3667,11 @@
         </c:dLbls>
         <c:gapWidth val="80"/>
         <c:overlap val="25"/>
-        <c:axId val="1848496591"/>
-        <c:axId val="1789200143"/>
+        <c:axId val="-1250756064"/>
+        <c:axId val="-1251063136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1848496591"/>
+        <c:axId val="-1250756064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3675,7 +3695,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -3694,7 +3714,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1789200143"/>
+        <c:crossAx val="-1251063136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3702,7 +3722,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1789200143"/>
+        <c:axId val="-1251063136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3753,7 +3773,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1848496591"/>
+        <c:crossAx val="-1250756064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3767,6 +3787,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3798,14 +3819,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -4934,7 +4955,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80B15F94-74E1-4AF2-8970-EB6B8F25ABC1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{80B15F94-74E1-4AF2-8970-EB6B8F25ABC1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4970,7 +4991,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9445A904-257A-4875-B69D-7F45EAF9FAEF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9445A904-257A-4875-B69D-7F45EAF9FAEF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5287,14 +5308,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6EF9586-F224-4D11-ADDF-4986AB86FE3B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W12" sqref="W12"/>
+    <sheetView tabSelected="1" topLeftCell="H4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="3.88671875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="61.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
@@ -5303,7 +5324,7 @@
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>38</v>
       </c>
@@ -5320,7 +5341,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -5337,7 +5358,7 @@
         <v>11.861000000000001</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
         <v>14</v>
       </c>
@@ -5354,7 +5375,7 @@
         <v>11.864000000000001</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
         <v>0</v>
       </c>
@@ -5371,7 +5392,7 @@
         <v>11.869</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
         <v>11</v>
       </c>
@@ -5388,7 +5409,7 @@
         <v>13.092000000000001</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -5405,7 +5426,7 @@
         <v>13.092000000000001</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
         <v>13</v>
       </c>
@@ -5422,7 +5443,7 @@
         <v>11.865</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -5439,7 +5460,7 @@
         <v>26.754999999999999</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
         <v>3</v>
       </c>
@@ -5456,7 +5477,7 @@
         <v>13.843</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
         <v>17</v>
       </c>
@@ -5473,7 +5494,7 @@
         <v>26.626999999999999</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
         <v>10</v>
       </c>
@@ -5490,7 +5511,7 @@
         <v>27.782</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B13" t="s">
         <v>9</v>
       </c>
@@ -5507,7 +5528,7 @@
         <v>28.007999999999999</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
         <v>5</v>
       </c>
@@ -5524,7 +5545,7 @@
         <v>26.754999999999999</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
         <v>16</v>
       </c>
@@ -5541,7 +5562,7 @@
         <v>26.754999999999999</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
         <v>8</v>
       </c>
@@ -5558,7 +5579,7 @@
         <v>16.675999999999998</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B17" t="s">
         <v>2</v>
       </c>
@@ -5575,7 +5596,7 @@
         <v>27.143000000000001</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B18" t="s">
         <v>1</v>
       </c>
@@ -5592,7 +5613,7 @@
         <v>29.706</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B19" t="s">
         <v>15</v>
       </c>
@@ -5609,7 +5630,7 @@
         <v>36.951000000000001</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B20" t="s">
         <v>18</v>
       </c>
@@ -5626,7 +5647,7 @@
         <v>43.68</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B21" t="s">
         <v>7</v>
       </c>
@@ -5643,7 +5664,7 @@
         <v>39.61</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B23" s="1" t="s">
         <v>38</v>
       </c>
@@ -5651,7 +5672,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
         <v>12</v>
       </c>
@@ -5659,7 +5680,7 @@
         <v>26.754999999999999</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B25" t="s">
         <v>14</v>
       </c>
@@ -5667,7 +5688,7 @@
         <v>27.143000000000001</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B26" t="s">
         <v>0</v>
       </c>
@@ -5675,7 +5696,7 @@
         <v>11.861000000000001</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B27" t="s">
         <v>11</v>
       </c>
@@ -5683,7 +5704,7 @@
         <v>26.754999999999999</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B28" t="s">
         <v>6</v>
       </c>
@@ -5691,7 +5712,7 @@
         <v>26.754999999999999</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
         <v>13</v>
       </c>
@@ -5699,7 +5720,7 @@
         <v>16.675999999999998</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B30" t="s">
         <v>4</v>
       </c>
@@ -5707,7 +5728,7 @@
         <v>13.092000000000001</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B31" t="s">
         <v>3</v>
       </c>
@@ -5715,7 +5736,7 @@
         <v>13.092000000000001</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B32" t="s">
         <v>17</v>
       </c>
@@ -5723,7 +5744,7 @@
         <v>43.68</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B33" t="s">
         <v>10</v>
       </c>
@@ -5731,7 +5752,7 @@
         <v>28.007999999999999</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B34" t="s">
         <v>9</v>
       </c>
@@ -5739,7 +5760,7 @@
         <v>27.782</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B35" t="s">
         <v>5</v>
       </c>
@@ -5747,7 +5768,7 @@
         <v>11.865</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B36" t="s">
         <v>16</v>
       </c>
@@ -5755,7 +5776,7 @@
         <v>36.951000000000001</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B37" t="s">
         <v>8</v>
       </c>
@@ -5763,7 +5784,7 @@
         <v>26.626999999999999</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B38" t="s">
         <v>2</v>
       </c>
@@ -5771,7 +5792,7 @@
         <v>11.869</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B39" t="s">
         <v>1</v>
       </c>
@@ -5779,7 +5800,7 @@
         <v>11.864000000000001</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B40" t="s">
         <v>15</v>
       </c>
@@ -5787,7 +5808,7 @@
         <v>29.706</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B41" t="s">
         <v>18</v>
       </c>
@@ -5795,7 +5816,7 @@
         <v>39.61</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B42" t="s">
         <v>7</v>
       </c>
@@ -5804,7 +5825,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F3:H21">
+  <sortState ref="F3:H21">
     <sortCondition ref="G3:G21"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5814,6 +5835,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003DB59D54AAC4B24EA9A98B6159AEDD81" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a776c128c0314cb3d9aae2760f8fd3ed">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a97ded03-527c-4a0c-b158-f2940a76ab81" xmlns:ns4="a35486a1-8de9-475b-b6e0-d65b6b15b04d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a509177177e4963985278f96f91598b3" ns3:_="" ns4:_="">
     <xsd:import namespace="a97ded03-527c-4a0c-b158-f2940a76ab81"/>
@@ -6036,15 +6066,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -6052,6 +6073,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6DAE986B-EB8C-45F5-81CA-F200183CDC61}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32778BE5-BD41-4D93-AA7F-37C8F944F48B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6066,14 +6095,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6DAE986B-EB8C-45F5-81CA-F200183CDC61}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Added the latest ORM Statistics result.
</commit_message>
<xml_diff>
--- a/assets/ORM Statistics Official Result.xlsx
+++ b/assets/ORM Statistics Official Result.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Entries" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,24 +30,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="40">
   <si>
     <t xml:space="preserve">Handcoded materializer using DbDataReader                            </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RepoDb (RawSql) v1.10.11.4                                           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RepoDb (Poco) v1.10.11.4                                             </t>
-  </si>
-  <si>
-    <t xml:space="preserve">LINQ to DB v2.9.7.0 (v2.9.7) (normal)                                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">LINQ to DB v2.9.7.0 (v2.9.7) (compiled)                              </t>
-  </si>
-  <si>
-    <t xml:space="preserve">LLBLGen Pro v5.6.0.0 (v5.6.2), Poco with Raw SQL                     </t>
   </si>
   <si>
     <t xml:space="preserve">Handcoded materializer using DbDataReader (GetValues(array), boxing) </t>
@@ -59,12 +44,6 @@
     <t xml:space="preserve">Raw DbDataReader materializer using object arrays                    </t>
   </si>
   <si>
-    <t xml:space="preserve">LLBLGen Pro v5.6.0.0 (v5.6.2), Poco typed view with QuerySpec        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">LLBLGen Pro v5.6.0.0 (v5.6.2), Poco typed view with Linq             </t>
-  </si>
-  <si>
     <t>Handcoded materializer using DbDataReader (GetValue(Ordinal), boxing)</t>
   </si>
   <si>
@@ -74,76 +53,13 @@
     <t xml:space="preserve">Handcoded materializer using DbDataReader and GetFieldValue&lt;T&gt;       </t>
   </si>
   <si>
-    <t xml:space="preserve">Entity Framework Core v3.1.3.0 (v3.100.320.12804)                    </t>
-  </si>
-  <si>
     <t xml:space="preserve">ServiceStack OrmLite v5.0.0.0 (v5.0.0.0)                             </t>
   </si>
   <si>
     <t xml:space="preserve">NPoco v4.0.2.0 (v4.0.2.0)                                            </t>
   </si>
   <si>
-    <t xml:space="preserve">LLBLGen Pro v5.6.0.0 (v5.6.2), DataTable based TypedView             </t>
-  </si>
-  <si>
     <t xml:space="preserve">Tortuga Chain v3.3.2.0                                               </t>
-  </si>
-  <si>
-    <t xml:space="preserve">75,79 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">76,12 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">78,54 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">78,62 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">80,45 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">82,65 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">86,29 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">87,57 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">89,18 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">90,96 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">92,80 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">94,40 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">96,96 </t>
-  </si>
-  <si>
-    <t>102,58</t>
-  </si>
-  <si>
-    <t>104,11</t>
-  </si>
-  <si>
-    <t>106,98</t>
-  </si>
-  <si>
-    <t>111,97</t>
-  </si>
-  <si>
-    <t>156,63</t>
-  </si>
-  <si>
-    <t>178,16</t>
   </si>
   <si>
     <t>ORM Framework</t>
@@ -155,10 +71,85 @@
     <t>In KB</t>
   </si>
   <si>
-    <t>Kilobytes</t>
+    <t xml:space="preserve">LINQ to DB v3.0.1.0 (v3.0.1) (normal)                                </t>
   </si>
   <si>
-    <t>Milliseconds</t>
+    <t xml:space="preserve">RepoDb (RawSql) v1.11.5.0                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RepoDb (Poco) v1.11.5.0                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LLBLGen Pro v5.7.0.0 (v5.7.0), Poco with Raw SQL                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LLBLGen Pro v5.7.0.0 (v5.7.0), Poco typed view with Linq             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LLBLGen Pro v5.7.0.0 (v5.7.0), Poco typed view with QuerySpec        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entity Framework Core v3.1.6.0 (v3.100.620.31702)                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LLBLGen Pro v5.7.0.0 (v5.7.0), DataTable based TypedView             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">76,84 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">83,41 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">83,96 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">84,65 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">87,25 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">87,84 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">89,76 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">91,38 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">98,20 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">98,31 </t>
+  </si>
+  <si>
+    <t>100,02</t>
+  </si>
+  <si>
+    <t>102,55</t>
+  </si>
+  <si>
+    <t>103,93</t>
+  </si>
+  <si>
+    <t>118,34</t>
+  </si>
+  <si>
+    <t>118,85</t>
+  </si>
+  <si>
+    <t>122,27</t>
+  </si>
+  <si>
+    <t>161,38</t>
+  </si>
+  <si>
+    <t>189,24</t>
+  </si>
+  <si>
+    <t>In MB</t>
   </si>
 </sst>
 </file>
@@ -200,9 +191,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,7 +424,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Milliseconds</c:v>
+                  <c:v>In MS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -441,7 +436,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>75.790000000000006</c:v>
+                  <c:v>76.84</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -461,7 +456,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>RepoDb (RawSql) v1.10.11.4                                           </c:v>
+                  <c:v>LINQ to DB v3.0.1.0 (v3.0.1) (normal)                                </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -570,7 +565,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Milliseconds</c:v>
+                  <c:v>In MS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -582,7 +577,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>76.12</c:v>
+                  <c:v>83.41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -602,7 +597,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>RepoDb (Poco) v1.10.11.4                                             </c:v>
+                  <c:v>RepoDb (RawSql) v1.11.5.0                                            </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -711,7 +706,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Milliseconds</c:v>
+                  <c:v>In MS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -723,7 +718,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>78.540000000000006</c:v>
+                  <c:v>83.96</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -743,7 +738,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>LINQ to DB v2.9.7.0 (v2.9.7) (normal)                                </c:v>
+                  <c:v>RepoDb (Poco) v1.11.5.0                                              </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -852,7 +847,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Milliseconds</c:v>
+                  <c:v>In MS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -864,7 +859,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>78.62</c:v>
+                  <c:v>84.65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -884,7 +879,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>LINQ to DB v2.9.7.0 (v2.9.7) (compiled)                              </c:v>
+                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.0), Poco with Raw SQL                     </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -993,7 +988,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Milliseconds</c:v>
+                  <c:v>In MS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1005,7 +1000,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>80.45</c:v>
+                  <c:v>87.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1025,7 +1020,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>LLBLGen Pro v5.6.0.0 (v5.6.2), Poco with Raw SQL                     </c:v>
+                  <c:v>Handcoded materializer using DbDataReader (GetValues(array), boxing) </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1134,7 +1129,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Milliseconds</c:v>
+                  <c:v>In MS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1146,7 +1141,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>82.65</c:v>
+                  <c:v>87.84</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1166,7 +1161,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Handcoded materializer using DbDataReader (GetValues(array), boxing) </c:v>
+                  <c:v>Tortuga Chain, Compiled v3.3.2.0                                     </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1278,7 +1273,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Milliseconds</c:v>
+                  <c:v>In MS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1290,7 +1285,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>86.29</c:v>
+                  <c:v>89.76</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1310,7 +1305,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Tortuga Chain, Compiled v3.3.2.0                                     </c:v>
+                  <c:v>Raw DbDataReader materializer using object arrays                    </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1422,7 +1417,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Milliseconds</c:v>
+                  <c:v>In MS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1434,7 +1429,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>87.57</c:v>
+                  <c:v>91.38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1454,7 +1449,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Raw DbDataReader materializer using object arrays                    </c:v>
+                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.0), Poco typed view with Linq             </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1566,7 +1561,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Milliseconds</c:v>
+                  <c:v>In MS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1578,7 +1573,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>89.18</c:v>
+                  <c:v>98.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1598,7 +1593,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>LLBLGen Pro v5.6.0.0 (v5.6.2), Poco typed view with QuerySpec        </c:v>
+                  <c:v>Handcoded materializer using DbDataReader (GetValue(Ordinal), boxing)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1710,7 +1705,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Milliseconds</c:v>
+                  <c:v>In MS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1722,7 +1717,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>90.96</c:v>
+                  <c:v>98.31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1742,7 +1737,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>LLBLGen Pro v5.6.0.0 (v5.6.2), Poco typed view with Linq             </c:v>
+                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.0), Poco typed view with QuerySpec        </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1854,7 +1849,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Milliseconds</c:v>
+                  <c:v>In MS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1866,7 +1861,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>92.8</c:v>
+                  <c:v>100.02</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1886,7 +1881,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Handcoded materializer using DbDataReader (GetValue(Ordinal), boxing)</c:v>
+                  <c:v>Entity Framework Core v3.1.6.0 (v3.100.620.31702)                    </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1998,7 +1993,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Milliseconds</c:v>
+                  <c:v>In MS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2010,7 +2005,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>94.4</c:v>
+                  <c:v>102.55</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2145,7 +2140,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Milliseconds</c:v>
+                  <c:v>In MS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2157,7 +2152,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>96.96</c:v>
+                  <c:v>103.93</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2177,7 +2172,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Handcoded materializer using DbDataReader and GetFieldValue&lt;T&gt;       </c:v>
+                  <c:v>NPoco v4.0.2.0 (v4.0.2.0)                                            </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2292,7 +2287,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Milliseconds</c:v>
+                  <c:v>In MS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2304,7 +2299,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>102.58</c:v>
+                  <c:v>118.34</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2324,7 +2319,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Entity Framework Core v3.1.3.0 (v3.100.320.12804)                    </c:v>
+                  <c:v>ServiceStack OrmLite v5.0.0.0 (v5.0.0.0)                             </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2439,7 +2434,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Milliseconds</c:v>
+                  <c:v>In MS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2451,7 +2446,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>104.11</c:v>
+                  <c:v>118.85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2471,7 +2466,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ServiceStack OrmLite v5.0.0.0 (v5.0.0.0)                             </c:v>
+                  <c:v>Handcoded materializer using DbDataReader and GetFieldValue&lt;T&gt;       </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2586,7 +2581,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Milliseconds</c:v>
+                  <c:v>In MS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2598,7 +2593,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>106.98</c:v>
+                  <c:v>122.27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2618,7 +2613,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>NPoco v4.0.2.0 (v4.0.2.0)                                            </c:v>
+                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.0), DataTable based TypedView             </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2733,7 +2728,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Milliseconds</c:v>
+                  <c:v>In MS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2745,7 +2740,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>111.97</c:v>
+                  <c:v>161.38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2765,7 +2760,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>LLBLGen Pro v5.6.0.0 (v5.6.2), DataTable based TypedView             </c:v>
+                  <c:v>Tortuga Chain v3.3.2.0                                               </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2880,7 +2875,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Milliseconds</c:v>
+                  <c:v>In MS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2892,7 +2887,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>156.63</c:v>
+                  <c:v>189.24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2911,9 +2906,6 @@
               <c:f>Entries!$F$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Tortuga Chain v3.3.2.0                                               </c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -3024,7 +3016,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Milliseconds</c:v>
+                  <c:v>In MS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3035,9 +3027,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>178.16</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3058,11 +3047,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="-1250758240"/>
-        <c:axId val="-1250752800"/>
+        <c:axId val="798251616"/>
+        <c:axId val="798252704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1250758240"/>
+        <c:axId val="798251616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3105,7 +3094,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1250752800"/>
+        <c:crossAx val="798252704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3113,7 +3102,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1250752800"/>
+        <c:axId val="798252704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3164,7 +3153,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1250758240"/>
+        <c:crossAx val="798251616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3340,7 +3329,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Milliseconds</c:v>
+                  <c:v>In MS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3359,64 +3348,61 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Entries!$F$3:$F$21</c:f>
+              <c:f>Entries!$F$3:$F$20</c:f>
               <c:strCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>Handcoded materializer using DbDataReader                            </c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>RepoDb (RawSql) v1.10.11.4                                           </c:v>
+                  <c:v>LINQ to DB v3.0.1.0 (v3.0.1) (normal)                                </c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>RepoDb (Poco) v1.10.11.4                                             </c:v>
+                  <c:v>RepoDb (RawSql) v1.11.5.0                                            </c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>LINQ to DB v2.9.7.0 (v2.9.7) (normal)                                </c:v>
+                  <c:v>RepoDb (Poco) v1.11.5.0                                              </c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>LINQ to DB v2.9.7.0 (v2.9.7) (compiled)                              </c:v>
+                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.0), Poco with Raw SQL                     </c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>LLBLGen Pro v5.6.0.0 (v5.6.2), Poco with Raw SQL                     </c:v>
+                  <c:v>Handcoded materializer using DbDataReader (GetValues(array), boxing) </c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Handcoded materializer using DbDataReader (GetValues(array), boxing) </c:v>
+                  <c:v>Tortuga Chain, Compiled v3.3.2.0                                     </c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Tortuga Chain, Compiled v3.3.2.0                                     </c:v>
+                  <c:v>Raw DbDataReader materializer using object arrays                    </c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Raw DbDataReader materializer using object arrays                    </c:v>
+                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.0), Poco typed view with Linq             </c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>LLBLGen Pro v5.6.0.0 (v5.6.2), Poco typed view with QuerySpec        </c:v>
+                  <c:v>Handcoded materializer using DbDataReader (GetValue(Ordinal), boxing)</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>LLBLGen Pro v5.6.0.0 (v5.6.2), Poco typed view with Linq             </c:v>
+                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.0), Poco typed view with QuerySpec        </c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Handcoded materializer using DbDataReader (GetValue(Ordinal), boxing)</c:v>
+                  <c:v>Entity Framework Core v3.1.6.0 (v3.100.620.31702)                    </c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>Dapper v2.0.0.0                                                      </c:v>
                 </c:pt>
                 <c:pt idx="13">
+                  <c:v>NPoco v4.0.2.0 (v4.0.2.0)                                            </c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>ServiceStack OrmLite v5.0.0.0 (v5.0.0.0)                             </c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>Handcoded materializer using DbDataReader and GetFieldValue&lt;T&gt;       </c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>Entity Framework Core v3.1.3.0 (v3.100.320.12804)                    </c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>ServiceStack OrmLite v5.0.0.0 (v5.0.0.0)                             </c:v>
-                </c:pt>
                 <c:pt idx="16">
-                  <c:v>NPoco v4.0.2.0 (v4.0.2.0)                                            </c:v>
+                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.0), DataTable based TypedView             </c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>LLBLGen Pro v5.6.0.0 (v5.6.2), DataTable based TypedView             </c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>Tortuga Chain v3.3.2.0                                               </c:v>
                 </c:pt>
               </c:strCache>
@@ -3424,66 +3410,63 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Entries!$G$3:$G$21</c:f>
+              <c:f>Entries!$G$3:$G$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>75.790000000000006</c:v>
+                  <c:v>76.84</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>76.12</c:v>
+                  <c:v>83.41</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>78.540000000000006</c:v>
+                  <c:v>83.96</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>78.62</c:v>
+                  <c:v>84.65</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>80.45</c:v>
+                  <c:v>87.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>82.65</c:v>
+                  <c:v>87.84</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>86.29</c:v>
+                  <c:v>89.76</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>87.57</c:v>
+                  <c:v>91.38</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>89.18</c:v>
+                  <c:v>98.2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>90.96</c:v>
+                  <c:v>98.31</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>92.8</c:v>
+                  <c:v>100.02</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>94.4</c:v>
+                  <c:v>102.55</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>96.96</c:v>
+                  <c:v>103.93</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>102.58</c:v>
+                  <c:v>118.34</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>104.11</c:v>
+                  <c:v>118.85</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>106.98</c:v>
+                  <c:v>122.27</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>111.97</c:v>
+                  <c:v>161.38</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>156.63</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>178.16</c:v>
+                  <c:v>189.24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3503,7 +3486,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Kilobytes</c:v>
+                  <c:v>In MB</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3522,64 +3505,61 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Entries!$F$3:$F$21</c:f>
+              <c:f>Entries!$F$3:$F$20</c:f>
               <c:strCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>Handcoded materializer using DbDataReader                            </c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>RepoDb (RawSql) v1.10.11.4                                           </c:v>
+                  <c:v>LINQ to DB v3.0.1.0 (v3.0.1) (normal)                                </c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>RepoDb (Poco) v1.10.11.4                                             </c:v>
+                  <c:v>RepoDb (RawSql) v1.11.5.0                                            </c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>LINQ to DB v2.9.7.0 (v2.9.7) (normal)                                </c:v>
+                  <c:v>RepoDb (Poco) v1.11.5.0                                              </c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>LINQ to DB v2.9.7.0 (v2.9.7) (compiled)                              </c:v>
+                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.0), Poco with Raw SQL                     </c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>LLBLGen Pro v5.6.0.0 (v5.6.2), Poco with Raw SQL                     </c:v>
+                  <c:v>Handcoded materializer using DbDataReader (GetValues(array), boxing) </c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Handcoded materializer using DbDataReader (GetValues(array), boxing) </c:v>
+                  <c:v>Tortuga Chain, Compiled v3.3.2.0                                     </c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Tortuga Chain, Compiled v3.3.2.0                                     </c:v>
+                  <c:v>Raw DbDataReader materializer using object arrays                    </c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Raw DbDataReader materializer using object arrays                    </c:v>
+                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.0), Poco typed view with Linq             </c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>LLBLGen Pro v5.6.0.0 (v5.6.2), Poco typed view with QuerySpec        </c:v>
+                  <c:v>Handcoded materializer using DbDataReader (GetValue(Ordinal), boxing)</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>LLBLGen Pro v5.6.0.0 (v5.6.2), Poco typed view with Linq             </c:v>
+                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.0), Poco typed view with QuerySpec        </c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Handcoded materializer using DbDataReader (GetValue(Ordinal), boxing)</c:v>
+                  <c:v>Entity Framework Core v3.1.6.0 (v3.100.620.31702)                    </c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>Dapper v2.0.0.0                                                      </c:v>
                 </c:pt>
                 <c:pt idx="13">
+                  <c:v>NPoco v4.0.2.0 (v4.0.2.0)                                            </c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>ServiceStack OrmLite v5.0.0.0 (v5.0.0.0)                             </c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>Handcoded materializer using DbDataReader and GetFieldValue&lt;T&gt;       </c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>Entity Framework Core v3.1.3.0 (v3.100.320.12804)                    </c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>ServiceStack OrmLite v5.0.0.0 (v5.0.0.0)                             </c:v>
-                </c:pt>
                 <c:pt idx="16">
-                  <c:v>NPoco v4.0.2.0 (v4.0.2.0)                                            </c:v>
+                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.0), DataTable based TypedView             </c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>LLBLGen Pro v5.6.0.0 (v5.6.2), DataTable based TypedView             </c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>Tortuga Chain v3.3.2.0                                               </c:v>
                 </c:pt>
               </c:strCache>
@@ -3587,66 +3567,63 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Entries!$H$3:$H$21</c:f>
+              <c:f>Entries!$H$3:$H$20</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>11.861000000000001</c:v>
+                  <c:v>11.5830078125</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.864000000000001</c:v>
+                  <c:v>12.06640625</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.869</c:v>
+                  <c:v>11.5849609375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13.092000000000001</c:v>
+                  <c:v>11.5859375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13.092000000000001</c:v>
+                  <c:v>11.5869140625</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11.865</c:v>
+                  <c:v>26.1279296875</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26.754999999999999</c:v>
+                  <c:v>13.5185546875</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13.843</c:v>
+                  <c:v>26.0029296875</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>26.626999999999999</c:v>
+                  <c:v>27.3515625</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>27.782</c:v>
+                  <c:v>26.1279296875</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>28.007999999999999</c:v>
+                  <c:v>27.130859375</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>26.754999999999999</c:v>
+                  <c:v>26.5068359375</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>26.754999999999999</c:v>
+                  <c:v>26.1279296875</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>16.675999999999998</c:v>
+                  <c:v>36.0849609375</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>27.143000000000001</c:v>
+                  <c:v>29.009765625</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>29.706</c:v>
+                  <c:v>16.28515625</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>36.951000000000001</c:v>
+                  <c:v>42.6591796875</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>43.68</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>39.61</c:v>
+                  <c:v>38.681640625</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3667,11 +3644,11 @@
         </c:dLbls>
         <c:gapWidth val="80"/>
         <c:overlap val="25"/>
-        <c:axId val="-1250756064"/>
-        <c:axId val="-1251063136"/>
+        <c:axId val="798239648"/>
+        <c:axId val="798232032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1250756064"/>
+        <c:axId val="798239648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3714,7 +3691,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1251063136"/>
+        <c:crossAx val="798232032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3722,7 +3699,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1251063136"/>
+        <c:axId val="798232032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3773,7 +3750,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1250756064"/>
+        <c:crossAx val="798239648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4945,7 +4922,7 @@
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>205740</xdr:colOff>
       <xdr:row>60</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
@@ -4955,7 +4932,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{80B15F94-74E1-4AF2-8970-EB6B8F25ABC1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80B15F94-74E1-4AF2-8970-EB6B8F25ABC1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4975,13 +4952,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>27</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>45720</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>65</xdr:col>
+      <xdr:col>66</xdr:col>
       <xdr:colOff>220980</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -4991,7 +4968,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9445A904-257A-4875-B69D-7F45EAF9FAEF}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9445A904-257A-4875-B69D-7F45EAF9FAEF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5309,524 +5286,575 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H42"/>
+  <dimension ref="B2:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="BV19" sqref="BV19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.88671875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="3.77734375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="61.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="61.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="60.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.71875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="1" t="s">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>41</v>
+      <c r="I2" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>75.790000000000006</v>
-      </c>
-      <c r="H3">
-        <v>11.861000000000001</v>
+        <v>76.84</v>
+      </c>
+      <c r="H3" s="2">
+        <f>I3/1024</f>
+        <v>11.5830078125</v>
+      </c>
+      <c r="I3" s="1">
+        <v>11861</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>
       </c>
       <c r="F4" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="G4">
-        <v>76.12</v>
-      </c>
-      <c r="H4">
-        <v>11.864000000000001</v>
+        <v>83.41</v>
+      </c>
+      <c r="H4" s="2">
+        <f t="shared" ref="H4:H20" si="0">I4/1024</f>
+        <v>12.06640625</v>
+      </c>
+      <c r="I4" s="1">
+        <v>12356</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="F5" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="G5">
-        <v>78.540000000000006</v>
-      </c>
-      <c r="H5">
-        <v>11.869</v>
+        <v>83.96</v>
+      </c>
+      <c r="H5" s="2">
+        <f t="shared" si="0"/>
+        <v>11.5849609375</v>
+      </c>
+      <c r="I5" s="1">
+        <v>11863</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
         <v>30</v>
       </c>
       <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6">
+        <v>84.65</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="0"/>
+        <v>11.5859375</v>
+      </c>
+      <c r="I6" s="1">
+        <v>11864</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7">
+        <v>87.25</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="0"/>
+        <v>11.5869140625</v>
+      </c>
+      <c r="I7" s="1">
+        <v>11865</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>87.84</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="0"/>
+        <v>26.1279296875</v>
+      </c>
+      <c r="I8" s="1">
+        <v>26755</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>89.76</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="0"/>
+        <v>13.5185546875</v>
+      </c>
+      <c r="I9" s="1">
+        <v>13843</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" t="s">
         <v>3</v>
       </c>
-      <c r="G6">
-        <v>78.62</v>
-      </c>
-      <c r="H6">
-        <v>13.092000000000001</v>
+      <c r="G10">
+        <v>91.38</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="0"/>
+        <v>26.0029296875</v>
+      </c>
+      <c r="I10" s="1">
+        <v>26627</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7">
-        <v>80.45</v>
-      </c>
-      <c r="H7">
-        <v>13.092000000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8">
-        <v>82.65</v>
-      </c>
-      <c r="H8">
-        <v>11.865</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9">
-        <v>86.29</v>
-      </c>
-      <c r="H9">
-        <v>26.754999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" t="s">
-        <v>7</v>
-      </c>
-      <c r="G10">
-        <v>87.57</v>
-      </c>
-      <c r="H10">
-        <v>13.843</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
         <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="F11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11">
+        <v>98.2</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="0"/>
+        <v>27.3515625</v>
+      </c>
+      <c r="I11" s="1">
+        <v>28008</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12">
+        <v>98.31</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="0"/>
+        <v>26.1279296875</v>
+      </c>
+      <c r="I12" s="1">
+        <v>26755</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13">
+        <v>100.02</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="0"/>
+        <v>27.130859375</v>
+      </c>
+      <c r="I13" s="1">
+        <v>27782</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B14" t="s">
         <v>8</v>
       </c>
-      <c r="G11">
-        <v>89.18</v>
-      </c>
-      <c r="H11">
-        <v>26.626999999999999</v>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14">
+        <v>102.55</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="0"/>
+        <v>26.5068359375</v>
+      </c>
+      <c r="I14" s="1">
+        <v>27143</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B12" t="s">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15">
+        <v>103.93</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="0"/>
+        <v>26.1279296875</v>
+      </c>
+      <c r="I15" s="1">
+        <v>26755</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16">
+        <v>118.34</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="0"/>
+        <v>36.0849609375</v>
+      </c>
+      <c r="I16" s="1">
+        <v>36951</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17">
+        <v>118.85</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="0"/>
+        <v>29.009765625</v>
+      </c>
+      <c r="I17" s="1">
+        <v>29706</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18">
+        <v>122.27</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" si="0"/>
+        <v>16.28515625</v>
+      </c>
+      <c r="I18" s="1">
+        <v>16676</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19">
+        <v>161.38</v>
+      </c>
+      <c r="H19" s="2">
+        <f t="shared" si="0"/>
+        <v>42.6591796875</v>
+      </c>
+      <c r="I19" s="1">
+        <v>43683</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20">
+        <v>189.24</v>
+      </c>
+      <c r="H20" s="2">
+        <f t="shared" si="0"/>
+        <v>38.681640625</v>
+      </c>
+      <c r="I20" s="1">
+        <v>39610</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B23" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C12" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12">
-        <v>90.96</v>
-      </c>
-      <c r="H12">
-        <v>27.782</v>
+      <c r="C23" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13">
-        <v>92.8</v>
-      </c>
-      <c r="H13">
-        <v>28.007999999999999</v>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>11.861000000000001</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B14" t="s">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B25" t="s">
         <v>5</v>
       </c>
-      <c r="C14" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14">
-        <v>94.4</v>
-      </c>
-      <c r="H14">
+      <c r="C25">
         <v>26.754999999999999</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15">
-        <v>96.96</v>
-      </c>
-      <c r="H15">
-        <v>26.754999999999999</v>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26">
+        <v>27.143000000000001</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16">
-        <v>102.58</v>
-      </c>
-      <c r="H16">
-        <v>16.675999999999998</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B17" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" t="s">
-        <v>21</v>
-      </c>
-      <c r="F17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17">
-        <v>104.11</v>
-      </c>
-      <c r="H17">
-        <v>27.143000000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" t="s">
-        <v>15</v>
-      </c>
-      <c r="G18">
-        <v>106.98</v>
-      </c>
-      <c r="H18">
-        <v>29.706</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" t="s">
-        <v>34</v>
-      </c>
-      <c r="F19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19">
-        <v>111.97</v>
-      </c>
-      <c r="H19">
-        <v>36.951000000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" t="s">
-        <v>37</v>
-      </c>
-      <c r="F20" t="s">
-        <v>17</v>
-      </c>
-      <c r="G20">
-        <v>156.63</v>
-      </c>
-      <c r="H20">
-        <v>43.68</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" t="s">
-        <v>26</v>
-      </c>
-      <c r="F21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G21">
-        <v>178.16</v>
-      </c>
-      <c r="H21">
-        <v>39.61</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B23" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24">
-        <v>26.754999999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B25" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25">
-        <v>27.143000000000001</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C26">
-        <v>11.861000000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B27" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C27">
         <v>26.754999999999999</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B28" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C28">
         <v>26.754999999999999</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C29">
         <v>16.675999999999998</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B30" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C30">
-        <v>13.092000000000001</v>
+        <v>12.356</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B31" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C31">
-        <v>13.092000000000001</v>
+        <v>43.683</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B32" t="s">
         <v>17</v>
       </c>
       <c r="C32">
-        <v>43.68</v>
+        <v>28.007999999999999</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B33" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C33">
-        <v>28.007999999999999</v>
+        <v>27.782</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B34" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C34">
-        <v>27.782</v>
+        <v>11.865</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B35" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C35">
-        <v>11.865</v>
+        <v>36.951000000000001</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B36" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C36">
-        <v>36.951000000000001</v>
+        <v>26.626999999999999</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B37" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C37">
-        <v>26.626999999999999</v>
+        <v>11.864000000000001</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B38" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C38">
-        <v>11.869</v>
+        <v>11.863</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B39" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C39">
-        <v>11.864000000000001</v>
+        <v>29.706</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B40" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C40">
-        <v>29.706</v>
+        <v>39.61</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B41" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C41">
-        <v>39.61</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B42" t="s">
-        <v>7</v>
-      </c>
-      <c r="C42">
         <v>13.843</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="F3:H21">
-    <sortCondition ref="G3:G21"/>
+  <sortState ref="F3:H20">
+    <sortCondition ref="G3:G20"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5835,15 +5863,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003DB59D54AAC4B24EA9A98B6159AEDD81" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a776c128c0314cb3d9aae2760f8fd3ed">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a97ded03-527c-4a0c-b158-f2940a76ab81" xmlns:ns4="a35486a1-8de9-475b-b6e0-d65b6b15b04d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a509177177e4963985278f96f91598b3" ns3:_="" ns4:_="">
     <xsd:import namespace="a97ded03-527c-4a0c-b158-f2940a76ab81"/>
@@ -6066,6 +6085,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -6073,14 +6101,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6DAE986B-EB8C-45F5-81CA-F200183CDC61}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32778BE5-BD41-4D93-AA7F-37C8F944F48B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6095,6 +6115,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6DAE986B-EB8C-45F5-81CA-F200183CDC61}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Updated the ORM Statistics Result.
</commit_message>
<xml_diff>
--- a/assets/ORM Statistics Official Result.xlsx
+++ b/assets/ORM Statistics Official Result.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="22">
   <si>
     <t xml:space="preserve">Handcoded materializer using DbDataReader                            </t>
   </si>
@@ -71,85 +71,31 @@
     <t>In KB</t>
   </si>
   <si>
-    <t xml:space="preserve">LINQ to DB v3.0.1.0 (v3.0.1) (normal)                                </t>
+    <t>In MB</t>
   </si>
   <si>
-    <t xml:space="preserve">RepoDb (RawSql) v1.11.5.0                                            </t>
+    <t xml:space="preserve">RepoDB (Raw-SQL) v1.12.0.5                                           </t>
   </si>
   <si>
-    <t xml:space="preserve">RepoDb (Poco) v1.11.5.0                                              </t>
+    <t xml:space="preserve">RepoDB (POCO) v1.12.0.5                                              </t>
   </si>
   <si>
-    <t xml:space="preserve">LLBLGen Pro v5.7.0.0 (v5.7.0), Poco with Raw SQL                     </t>
+    <t xml:space="preserve">LINQ to DB v3.1.3.0 (v3.1.3) (normal)                                </t>
   </si>
   <si>
-    <t xml:space="preserve">LLBLGen Pro v5.7.0.0 (v5.7.0), Poco typed view with Linq             </t>
+    <t xml:space="preserve">LLBLGen Pro v5.7.0.0 (v5.7.1), Poco with Raw SQL                     </t>
   </si>
   <si>
-    <t xml:space="preserve">LLBLGen Pro v5.7.0.0 (v5.7.0), Poco typed view with QuerySpec        </t>
+    <t xml:space="preserve">LLBLGen Pro v5.7.0.0 (v5.7.1), Poco typed view with QuerySpec        </t>
   </si>
   <si>
-    <t xml:space="preserve">Entity Framework Core v3.1.6.0 (v3.100.620.31702)                    </t>
+    <t xml:space="preserve">LLBLGen Pro v5.7.0.0 (v5.7.1), Poco typed view with Linq             </t>
   </si>
   <si>
-    <t xml:space="preserve">LLBLGen Pro v5.7.0.0 (v5.7.0), DataTable based TypedView             </t>
+    <t xml:space="preserve">Entity Framework Core v3.1.8.0 (v3.100.820.42012)                    </t>
   </si>
   <si>
-    <t xml:space="preserve">76,84 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">83,41 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">83,96 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">84,65 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">87,25 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">87,84 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">89,76 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">91,38 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">98,20 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">98,31 </t>
-  </si>
-  <si>
-    <t>100,02</t>
-  </si>
-  <si>
-    <t>102,55</t>
-  </si>
-  <si>
-    <t>103,93</t>
-  </si>
-  <si>
-    <t>118,34</t>
-  </si>
-  <si>
-    <t>118,85</t>
-  </si>
-  <si>
-    <t>122,27</t>
-  </si>
-  <si>
-    <t>161,38</t>
-  </si>
-  <si>
-    <t>189,24</t>
-  </si>
-  <si>
-    <t>In MB</t>
+    <t xml:space="preserve">LLBLGen Pro v5.7.0.0 (v5.7.1), DataTable based TypedView             </t>
   </si>
 </sst>
 </file>
@@ -436,7 +382,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>76.84</c:v>
+                  <c:v>77.36</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -456,7 +402,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>LINQ to DB v3.0.1.0 (v3.0.1) (normal)                                </c:v>
+                  <c:v>RepoDB (Raw-SQL) v1.12.0.5                                           </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -577,7 +523,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>83.41</c:v>
+                  <c:v>77.77</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -597,7 +543,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>RepoDb (RawSql) v1.11.5.0                                            </c:v>
+                  <c:v>RepoDB (POCO) v1.12.0.5                                              </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -718,7 +664,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>83.96</c:v>
+                  <c:v>79.540000000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -738,7 +684,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>RepoDb (Poco) v1.11.5.0                                              </c:v>
+                  <c:v>LINQ to DB v3.1.3.0 (v3.1.3) (normal)                                </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -859,7 +805,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>84.65</c:v>
+                  <c:v>83.02</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -879,7 +825,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.0), Poco with Raw SQL                     </c:v>
+                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.1), Poco with Raw SQL                     </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1000,7 +946,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>87.25</c:v>
+                  <c:v>86.39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1020,7 +966,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Handcoded materializer using DbDataReader (GetValues(array), boxing) </c:v>
+                  <c:v>Raw DbDataReader materializer using object arrays                    </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1141,7 +1087,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>87.84</c:v>
+                  <c:v>87.54</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1161,7 +1107,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Tortuga Chain, Compiled v3.3.2.0                                     </c:v>
+                  <c:v>Handcoded materializer using DbDataReader (GetValues(array), boxing) </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1285,7 +1231,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>89.76</c:v>
+                  <c:v>89.16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1305,7 +1251,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Raw DbDataReader materializer using object arrays                    </c:v>
+                  <c:v>Tortuga Chain, Compiled v3.3.2.0                                     </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1429,7 +1375,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>91.38</c:v>
+                  <c:v>92.24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1449,7 +1395,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.0), Poco typed view with Linq             </c:v>
+                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.1), Poco typed view with QuerySpec        </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1573,7 +1519,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>98.2</c:v>
+                  <c:v>96.58</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1593,7 +1539,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Handcoded materializer using DbDataReader (GetValue(Ordinal), boxing)</c:v>
+                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.1), Poco typed view with Linq             </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1717,7 +1663,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>98.31</c:v>
+                  <c:v>98.47</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1737,7 +1683,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.0), Poco typed view with QuerySpec        </c:v>
+                  <c:v>Handcoded materializer using DbDataReader (GetValue(Ordinal), boxing)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1861,7 +1807,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>100.02</c:v>
+                  <c:v>99.33</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1881,7 +1827,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Entity Framework Core v3.1.6.0 (v3.100.620.31702)                    </c:v>
+                  <c:v>Dapper v2.0.0.0                                                      </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2005,7 +1951,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>102.55</c:v>
+                  <c:v>103.92</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2025,7 +1971,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Dapper v2.0.0.0                                                      </c:v>
+                  <c:v>Entity Framework Core v3.1.8.0 (v3.100.820.42012)                    </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2152,7 +2098,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>103.93</c:v>
+                  <c:v>107.93</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2299,7 +2245,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>118.34</c:v>
+                  <c:v>116.19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2319,7 +2265,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ServiceStack OrmLite v5.0.0.0 (v5.0.0.0)                             </c:v>
+                  <c:v>Handcoded materializer using DbDataReader and GetFieldValue&lt;T&gt;       </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2446,7 +2392,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>118.85</c:v>
+                  <c:v>116.63</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2466,7 +2412,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Handcoded materializer using DbDataReader and GetFieldValue&lt;T&gt;       </c:v>
+                  <c:v>ServiceStack OrmLite v5.0.0.0 (v5.0.0.0)                             </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2593,7 +2539,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>122.27</c:v>
+                  <c:v>118.72</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2613,7 +2559,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.0), DataTable based TypedView             </c:v>
+                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.1), DataTable based TypedView             </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2740,7 +2686,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>161.38</c:v>
+                  <c:v>165.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2887,7 +2833,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>189.24</c:v>
+                  <c:v>190.85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2991,7 +2937,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3047,11 +2992,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="798251616"/>
-        <c:axId val="798252704"/>
+        <c:axId val="1087893440"/>
+        <c:axId val="1087893984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="798251616"/>
+        <c:axId val="1087893440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3094,7 +3039,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="798252704"/>
+        <c:crossAx val="1087893984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3102,7 +3047,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="798252704"/>
+        <c:axId val="1087893984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3153,7 +3098,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="798251616"/>
+        <c:crossAx val="1087893440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3355,52 +3300,52 @@
                   <c:v>Handcoded materializer using DbDataReader                            </c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>LINQ to DB v3.0.1.0 (v3.0.1) (normal)                                </c:v>
+                  <c:v>RepoDB (Raw-SQL) v1.12.0.5                                           </c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>RepoDb (RawSql) v1.11.5.0                                            </c:v>
+                  <c:v>RepoDB (POCO) v1.12.0.5                                              </c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>RepoDb (Poco) v1.11.5.0                                              </c:v>
+                  <c:v>LINQ to DB v3.1.3.0 (v3.1.3) (normal)                                </c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.0), Poco with Raw SQL                     </c:v>
+                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.1), Poco with Raw SQL                     </c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>Raw DbDataReader materializer using object arrays                    </c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>Handcoded materializer using DbDataReader (GetValues(array), boxing) </c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Tortuga Chain, Compiled v3.3.2.0                                     </c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>Raw DbDataReader materializer using object arrays                    </c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.0), Poco typed view with Linq             </c:v>
+                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.1), Poco typed view with QuerySpec        </c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.1), Poco typed view with Linq             </c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>Handcoded materializer using DbDataReader (GetValue(Ordinal), boxing)</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.0), Poco typed view with QuerySpec        </c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>Entity Framework Core v3.1.6.0 (v3.100.620.31702)                    </c:v>
+                  <c:v>Dapper v2.0.0.0                                                      </c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Dapper v2.0.0.0                                                      </c:v>
+                  <c:v>Entity Framework Core v3.1.8.0 (v3.100.820.42012)                    </c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>NPoco v4.0.2.0 (v4.0.2.0)                                            </c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>Handcoded materializer using DbDataReader and GetFieldValue&lt;T&gt;       </c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>ServiceStack OrmLite v5.0.0.0 (v5.0.0.0)                             </c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>Handcoded materializer using DbDataReader and GetFieldValue&lt;T&gt;       </c:v>
-                </c:pt>
                 <c:pt idx="16">
-                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.0), DataTable based TypedView             </c:v>
+                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.1), DataTable based TypedView             </c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>Tortuga Chain v3.3.2.0                                               </c:v>
@@ -3415,58 +3360,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>76.84</c:v>
+                  <c:v>77.36</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>83.41</c:v>
+                  <c:v>77.77</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>83.96</c:v>
+                  <c:v>79.540000000000006</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>84.65</c:v>
+                  <c:v>83.02</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>87.25</c:v>
+                  <c:v>86.39</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>87.84</c:v>
+                  <c:v>87.54</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>89.76</c:v>
+                  <c:v>89.16</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>91.38</c:v>
+                  <c:v>92.24</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>98.2</c:v>
+                  <c:v>96.58</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>98.31</c:v>
+                  <c:v>98.47</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>100.02</c:v>
+                  <c:v>99.33</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>102.55</c:v>
+                  <c:v>103.92</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>103.93</c:v>
+                  <c:v>107.93</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>118.34</c:v>
+                  <c:v>116.19</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>118.85</c:v>
+                  <c:v>116.63</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>122.27</c:v>
+                  <c:v>118.72</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>161.38</c:v>
+                  <c:v>165.75</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>189.24</c:v>
+                  <c:v>190.85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3512,52 +3457,52 @@
                   <c:v>Handcoded materializer using DbDataReader                            </c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>LINQ to DB v3.0.1.0 (v3.0.1) (normal)                                </c:v>
+                  <c:v>RepoDB (Raw-SQL) v1.12.0.5                                           </c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>RepoDb (RawSql) v1.11.5.0                                            </c:v>
+                  <c:v>RepoDB (POCO) v1.12.0.5                                              </c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>RepoDb (Poco) v1.11.5.0                                              </c:v>
+                  <c:v>LINQ to DB v3.1.3.0 (v3.1.3) (normal)                                </c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.0), Poco with Raw SQL                     </c:v>
+                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.1), Poco with Raw SQL                     </c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>Raw DbDataReader materializer using object arrays                    </c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>Handcoded materializer using DbDataReader (GetValues(array), boxing) </c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Tortuga Chain, Compiled v3.3.2.0                                     </c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>Raw DbDataReader materializer using object arrays                    </c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.0), Poco typed view with Linq             </c:v>
+                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.1), Poco typed view with QuerySpec        </c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.1), Poco typed view with Linq             </c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>Handcoded materializer using DbDataReader (GetValue(Ordinal), boxing)</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.0), Poco typed view with QuerySpec        </c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>Entity Framework Core v3.1.6.0 (v3.100.620.31702)                    </c:v>
+                  <c:v>Dapper v2.0.0.0                                                      </c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Dapper v2.0.0.0                                                      </c:v>
+                  <c:v>Entity Framework Core v3.1.8.0 (v3.100.820.42012)                    </c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>NPoco v4.0.2.0 (v4.0.2.0)                                            </c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>Handcoded materializer using DbDataReader and GetFieldValue&lt;T&gt;       </c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>ServiceStack OrmLite v5.0.0.0 (v5.0.0.0)                             </c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>Handcoded materializer using DbDataReader and GetFieldValue&lt;T&gt;       </c:v>
-                </c:pt>
                 <c:pt idx="16">
-                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.0), DataTable based TypedView             </c:v>
+                  <c:v>LLBLGen Pro v5.7.0.0 (v5.7.1), DataTable based TypedView             </c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>Tortuga Chain v3.3.2.0                                               </c:v>
@@ -3575,49 +3520,49 @@
                   <c:v>11.5830078125</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.06640625</c:v>
+                  <c:v>11.5830078125</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.5849609375</c:v>
+                  <c:v>11.583984375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.5859375</c:v>
+                  <c:v>12.0673828125</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>11.5869140625</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>26.0029296875</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>26.1279296875</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>13.5185546875</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>26.0029296875</c:v>
-                </c:pt>
                 <c:pt idx="8">
+                  <c:v>27.130859375</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>27.3515625</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>26.1279296875</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>27.130859375</c:v>
-                </c:pt>
                 <c:pt idx="11">
+                  <c:v>26.1279296875</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>26.5068359375</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>26.1279296875</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>36.0849609375</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>16.28515625</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>29.009765625</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16.28515625</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>42.6591796875</c:v>
@@ -3644,11 +3589,11 @@
         </c:dLbls>
         <c:gapWidth val="80"/>
         <c:overlap val="25"/>
-        <c:axId val="798239648"/>
-        <c:axId val="798232032"/>
+        <c:axId val="1087901600"/>
+        <c:axId val="1087883648"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="798239648"/>
+        <c:axId val="1087901600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3691,7 +3636,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="798232032"/>
+        <c:crossAx val="1087883648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3699,7 +3644,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="798232032"/>
+        <c:axId val="1087883648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3750,7 +3695,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="798239648"/>
+        <c:crossAx val="1087901600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4932,7 +4877,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80B15F94-74E1-4AF2-8970-EB6B8F25ABC1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{80B15F94-74E1-4AF2-8970-EB6B8F25ABC1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4955,20 +4900,20 @@
       <xdr:col>28</xdr:col>
       <xdr:colOff>45720</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>76199</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>66</xdr:col>
-      <xdr:colOff>220980</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>79</xdr:col>
+      <xdr:colOff>49306</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9445A904-257A-4875-B69D-7F45EAF9FAEF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9445A904-257A-4875-B69D-7F45EAF9FAEF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5288,8 +5233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="BV19" sqref="BV19"/>
+    <sheetView tabSelected="1" topLeftCell="Q10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BQ21" sqref="BQ21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.77734375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -5298,7 +5243,7 @@
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="60.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.71875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.71875" customWidth="1"/>
     <col min="9" max="9" width="6.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5316,7 +5261,7 @@
         <v>11</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>12</v>
@@ -5324,16 +5269,16 @@
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>103.92</v>
       </c>
       <c r="F3" t="s">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>76.84</v>
+        <v>77.36</v>
       </c>
       <c r="H3" s="2">
         <f>I3/1024</f>
@@ -5345,82 +5290,82 @@
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>33</v>
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>107.93</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G4">
-        <v>83.41</v>
+        <v>77.77</v>
       </c>
       <c r="H4" s="2">
-        <f t="shared" ref="H4:H20" si="0">I4/1024</f>
-        <v>12.06640625</v>
+        <f>I4/1024</f>
+        <v>11.5830078125</v>
       </c>
       <c r="I4" s="1">
-        <v>12356</v>
+        <v>11861</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>32</v>
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>77.36</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G5">
-        <v>83.96</v>
+        <v>79.540000000000006</v>
       </c>
       <c r="H5" s="2">
-        <f t="shared" si="0"/>
-        <v>11.5849609375</v>
+        <f>I5/1024</f>
+        <v>11.583984375</v>
       </c>
       <c r="I5" s="1">
-        <v>11863</v>
+        <v>11862</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
-        <v>30</v>
+      <c r="C6">
+        <v>99.33</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G6">
-        <v>84.65</v>
+        <v>83.02</v>
       </c>
       <c r="H6" s="2">
-        <f t="shared" si="0"/>
-        <v>11.5859375</v>
+        <f>I6/1024</f>
+        <v>12.0673828125</v>
       </c>
       <c r="I6" s="1">
-        <v>11864</v>
+        <v>12357</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
         <v>1</v>
       </c>
-      <c r="C7" t="s">
-        <v>26</v>
+      <c r="C7">
+        <v>89.16</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G7">
-        <v>87.25</v>
+        <v>86.39</v>
       </c>
       <c r="H7" s="2">
-        <f t="shared" si="0"/>
+        <f>I7/1024</f>
         <v>11.5869140625</v>
       </c>
       <c r="I7" s="1">
@@ -5431,185 +5376,185 @@
       <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
-        <v>36</v>
+      <c r="C8">
+        <v>116.63</v>
       </c>
       <c r="F8" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G8">
-        <v>87.84</v>
+        <v>87.54</v>
       </c>
       <c r="H8" s="2">
-        <f t="shared" si="0"/>
-        <v>26.1279296875</v>
+        <f>I8/1024</f>
+        <v>26.0029296875</v>
       </c>
       <c r="I8" s="1">
-        <v>26755</v>
+        <v>26627</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <v>83.02</v>
       </c>
       <c r="F9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9">
-        <v>89.76</v>
+        <v>89.16</v>
       </c>
       <c r="H9" s="2">
-        <f t="shared" si="0"/>
-        <v>13.5185546875</v>
+        <f>I9/1024</f>
+        <v>26.1279296875</v>
       </c>
       <c r="I9" s="1">
-        <v>13843</v>
+        <v>26755</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>37</v>
+        <v>21</v>
+      </c>
+      <c r="C10">
+        <v>165.75</v>
       </c>
       <c r="F10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G10">
-        <v>91.38</v>
+        <v>92.24</v>
       </c>
       <c r="H10" s="2">
-        <f t="shared" si="0"/>
-        <v>26.0029296875</v>
+        <f>I10/1024</f>
+        <v>13.5185546875</v>
       </c>
       <c r="I10" s="1">
-        <v>26627</v>
+        <v>13843</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>29</v>
+        <v>19</v>
+      </c>
+      <c r="C11">
+        <v>98.47</v>
       </c>
       <c r="F11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G11">
-        <v>98.2</v>
+        <v>96.58</v>
       </c>
       <c r="H11" s="2">
-        <f t="shared" si="0"/>
-        <v>27.3515625</v>
+        <f>I11/1024</f>
+        <v>27.130859375</v>
       </c>
       <c r="I11" s="1">
-        <v>28008</v>
+        <v>27782</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
         <v>18</v>
       </c>
-      <c r="C12" t="s">
-        <v>31</v>
+      <c r="C12">
+        <v>96.58</v>
       </c>
       <c r="F12" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="G12">
-        <v>98.31</v>
+        <v>98.47</v>
       </c>
       <c r="H12" s="2">
-        <f t="shared" si="0"/>
-        <v>26.1279296875</v>
+        <f>I12/1024</f>
+        <v>27.3515625</v>
       </c>
       <c r="I12" s="1">
-        <v>26755</v>
+        <v>28008</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" t="s">
-        <v>25</v>
+        <v>17</v>
+      </c>
+      <c r="C13">
+        <v>86.39</v>
       </c>
       <c r="F13" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="G13">
-        <v>100.02</v>
+        <v>99.33</v>
       </c>
       <c r="H13" s="2">
-        <f t="shared" si="0"/>
-        <v>27.130859375</v>
+        <f>I13/1024</f>
+        <v>26.1279296875</v>
       </c>
       <c r="I13" s="1">
-        <v>27782</v>
+        <v>26755</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
         <v>8</v>
       </c>
-      <c r="C14" t="s">
-        <v>34</v>
+      <c r="C14">
+        <v>116.19</v>
       </c>
       <c r="F14" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="G14">
-        <v>102.55</v>
+        <v>103.92</v>
       </c>
       <c r="H14" s="2">
-        <f t="shared" si="0"/>
-        <v>26.5068359375</v>
+        <f>I14/1024</f>
+        <v>26.1279296875</v>
       </c>
       <c r="I14" s="1">
-        <v>27143</v>
+        <v>26755</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
         <v>3</v>
       </c>
-      <c r="C15" t="s">
-        <v>28</v>
+      <c r="C15">
+        <v>87.54</v>
       </c>
       <c r="F15" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="G15">
-        <v>103.93</v>
+        <v>107.93</v>
       </c>
       <c r="H15" s="2">
-        <f t="shared" si="0"/>
-        <v>26.1279296875</v>
+        <f>I15/1024</f>
+        <v>26.5068359375</v>
       </c>
       <c r="I15" s="1">
-        <v>26755</v>
+        <v>27143</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
         <v>15</v>
       </c>
-      <c r="C16" t="s">
-        <v>24</v>
+      <c r="C16">
+        <v>79.540000000000006</v>
       </c>
       <c r="F16" t="s">
         <v>8</v>
       </c>
       <c r="G16">
-        <v>118.34</v>
+        <v>116.19</v>
       </c>
       <c r="H16" s="2">
-        <f t="shared" si="0"/>
+        <f>I16/1024</f>
         <v>36.0849609375</v>
       </c>
       <c r="I16" s="1">
@@ -5620,59 +5565,59 @@
       <c r="B17" t="s">
         <v>14</v>
       </c>
-      <c r="C17" t="s">
-        <v>23</v>
+      <c r="C17">
+        <v>77.77</v>
       </c>
       <c r="F17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G17">
-        <v>118.85</v>
+        <v>116.63</v>
       </c>
       <c r="H17" s="2">
-        <f t="shared" si="0"/>
-        <v>29.009765625</v>
+        <f>I17/1024</f>
+        <v>16.28515625</v>
       </c>
       <c r="I17" s="1">
-        <v>29706</v>
+        <v>16676</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B18" t="s">
         <v>7</v>
       </c>
-      <c r="C18" t="s">
-        <v>35</v>
+      <c r="C18">
+        <v>118.72</v>
       </c>
       <c r="F18" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G18">
-        <v>122.27</v>
+        <v>118.72</v>
       </c>
       <c r="H18" s="2">
-        <f t="shared" si="0"/>
-        <v>16.28515625</v>
+        <f>I18/1024</f>
+        <v>29.009765625</v>
       </c>
       <c r="I18" s="1">
-        <v>16676</v>
+        <v>29706</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B19" t="s">
         <v>9</v>
       </c>
-      <c r="C19" t="s">
-        <v>38</v>
+      <c r="C19">
+        <v>190.85</v>
       </c>
       <c r="F19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G19">
-        <v>161.38</v>
+        <v>165.75</v>
       </c>
       <c r="H19" s="2">
-        <f t="shared" si="0"/>
+        <f>I19/1024</f>
         <v>42.6591796875</v>
       </c>
       <c r="I19" s="1">
@@ -5683,17 +5628,17 @@
       <c r="B20" t="s">
         <v>2</v>
       </c>
-      <c r="C20" t="s">
-        <v>27</v>
+      <c r="C20">
+        <v>92.24</v>
       </c>
       <c r="F20" t="s">
         <v>9</v>
       </c>
       <c r="G20">
-        <v>189.24</v>
+        <v>190.85</v>
       </c>
       <c r="H20" s="2">
-        <f t="shared" si="0"/>
+        <f>I20/1024</f>
         <v>38.681640625</v>
       </c>
       <c r="I20" s="1">
@@ -5710,150 +5655,150 @@
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C24">
-        <v>11.861000000000001</v>
+        <v>5</v>
+      </c>
+      <c r="C24" s="1">
+        <v>26755</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25">
-        <v>26.754999999999999</v>
+        <v>20</v>
+      </c>
+      <c r="C25" s="1">
+        <v>27143</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B26" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26">
-        <v>27.143000000000001</v>
+        <v>0</v>
+      </c>
+      <c r="C26" s="1">
+        <v>11861</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B27" t="s">
         <v>4</v>
       </c>
-      <c r="C27">
-        <v>26.754999999999999</v>
+      <c r="C27" s="1">
+        <v>26755</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B28" t="s">
         <v>1</v>
       </c>
-      <c r="C28">
-        <v>26.754999999999999</v>
+      <c r="C28" s="1">
+        <v>26755</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
         <v>6</v>
       </c>
-      <c r="C29">
-        <v>16.675999999999998</v>
+      <c r="C29" s="1">
+        <v>16676</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B30" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30">
-        <v>12.356</v>
+        <v>16</v>
+      </c>
+      <c r="C30" s="1">
+        <v>12357</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B31" t="s">
-        <v>20</v>
-      </c>
-      <c r="C31">
-        <v>43.683</v>
+        <v>21</v>
+      </c>
+      <c r="C31" s="1">
+        <v>43683</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B32" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32">
-        <v>28.007999999999999</v>
+        <v>19</v>
+      </c>
+      <c r="C32" s="1">
+        <v>28008</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B33" t="s">
         <v>18</v>
       </c>
-      <c r="C33">
-        <v>27.782</v>
+      <c r="C33" s="1">
+        <v>27782</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B34" t="s">
-        <v>16</v>
-      </c>
-      <c r="C34">
-        <v>11.865</v>
+        <v>17</v>
+      </c>
+      <c r="C34" s="1">
+        <v>11865</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B35" t="s">
         <v>8</v>
       </c>
-      <c r="C35">
-        <v>36.951000000000001</v>
+      <c r="C35" s="1">
+        <v>36951</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B36" t="s">
         <v>3</v>
       </c>
-      <c r="C36">
-        <v>26.626999999999999</v>
+      <c r="C36" s="1">
+        <v>26627</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B37" t="s">
         <v>15</v>
       </c>
-      <c r="C37">
-        <v>11.864000000000001</v>
+      <c r="C37" s="1">
+        <v>11862</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B38" t="s">
         <v>14</v>
       </c>
-      <c r="C38">
-        <v>11.863</v>
+      <c r="C38" s="1">
+        <v>11861</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B39" t="s">
         <v>7</v>
       </c>
-      <c r="C39">
-        <v>29.706</v>
+      <c r="C39" s="1">
+        <v>29706</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B40" t="s">
         <v>9</v>
       </c>
-      <c r="C40">
-        <v>39.61</v>
+      <c r="C40" s="1">
+        <v>39610</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B41" t="s">
         <v>2</v>
       </c>
-      <c r="C41">
-        <v>13.843</v>
+      <c r="C41" s="1">
+        <v>13843</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="F3:H20">
+  <sortState ref="F3:I20">
     <sortCondition ref="G3:G20"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6086,18 +6031,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6120,14 +6065,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6DAE986B-EB8C-45F5-81CA-F200183CDC61}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1357F301-0B8B-4188-9FBA-2D28B749906F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -6142,4 +6079,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6DAE986B-EB8C-45F5-81CA-F200183CDC61}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated the ORM Statistics.
</commit_message>
<xml_diff>
--- a/assets/ORM Statistics Official Result.xlsx
+++ b/assets/ORM Statistics Official Result.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MichaelP\Source\Repos\GitHub\RepoDb.NET\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\GitHub\RepoDB.NET\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295B7EF3-FD85-45D3-9CB0-1974DAE94112}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-7440" windowWidth="38616" windowHeight="21360" tabRatio="538"/>
+    <workbookView xWindow="53892" yWindow="-108" windowWidth="25416" windowHeight="15516" tabRatio="538" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Entries" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -56,9 +59,6 @@
     <t xml:space="preserve">ServiceStack OrmLite v5.0.0.0 (v5.0.0.0)                             </t>
   </si>
   <si>
-    <t xml:space="preserve">NPoco v4.0.2.0 (v4.0.2.0)                                            </t>
-  </si>
-  <si>
     <t xml:space="preserve">Tortuga Chain v3.3.2.0                                               </t>
   </si>
   <si>
@@ -74,15 +74,6 @@
     <t>In MB</t>
   </si>
   <si>
-    <t xml:space="preserve">RepoDB (Raw-SQL) v1.12.0.5                                           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RepoDB (POCO) v1.12.0.5                                              </t>
-  </si>
-  <si>
-    <t xml:space="preserve">LINQ to DB v3.1.3.0 (v3.1.3) (normal)                                </t>
-  </si>
-  <si>
     <t xml:space="preserve">LLBLGen Pro v5.7.0.0 (v5.7.1), Poco with Raw SQL                     </t>
   </si>
   <si>
@@ -92,16 +83,28 @@
     <t xml:space="preserve">LLBLGen Pro v5.7.0.0 (v5.7.1), Poco typed view with Linq             </t>
   </si>
   <si>
-    <t xml:space="preserve">Entity Framework Core v3.1.8.0 (v3.100.820.42012)                    </t>
+    <t xml:space="preserve">LLBLGen Pro v5.7.0.0 (v5.7.1), DataTable based TypedView             </t>
   </si>
   <si>
-    <t xml:space="preserve">LLBLGen Pro v5.7.0.0 (v5.7.1), DataTable based TypedView             </t>
+    <t xml:space="preserve">RepoDB (Raw-SQL) v1.12.4.0                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RepoDB (POCO) v1.12.4.0                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LINQ to DB v3.1.6.0 (v3.1.6) (normal)                                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entity Framework Core v5.0.0.0 (v5.0.20.52303)                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NPoco v4.0.3.0 (v4.0.3.0)                                            </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -162,7 +165,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -215,7 +218,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -261,7 +263,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Handcoded materializer using DbDataReader                            </c:v>
+                  <c:v>RepoDB (Raw-SQL) v1.12.4.0                                           </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -343,9 +345,8 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -382,12 +383,12 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>77.36</c:v>
+                  <c:v>59.86</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -402,7 +403,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>RepoDB (Raw-SQL) v1.12.0.5                                           </c:v>
+                  <c:v>Handcoded materializer using DbDataReader                            </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -484,9 +485,8 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -523,12 +523,12 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>77.77</c:v>
+                  <c:v>60.55</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -543,7 +543,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>RepoDB (POCO) v1.12.0.5                                              </c:v>
+                  <c:v>RepoDB (POCO) v1.12.4.0                                              </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -625,9 +625,8 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -664,12 +663,12 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>79.540000000000006</c:v>
+                  <c:v>62.52</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -684,7 +683,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>LINQ to DB v3.1.3.0 (v3.1.3) (normal)                                </c:v>
+                  <c:v>LINQ to DB v3.1.6.0 (v3.1.6) (normal)                                </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -766,9 +765,8 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -805,12 +803,12 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>83.02</c:v>
+                  <c:v>65.02</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -907,9 +905,8 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -946,12 +943,12 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>86.39</c:v>
+                  <c:v>66.84</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -966,7 +963,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Raw DbDataReader materializer using object arrays                    </c:v>
+                  <c:v>Handcoded materializer using DbDataReader (GetValues(array), boxing) </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1048,9 +1045,8 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1087,12 +1083,12 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>87.54</c:v>
+                  <c:v>66.900000000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -1107,7 +1103,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Handcoded materializer using DbDataReader (GetValues(array), boxing) </c:v>
+                  <c:v>Raw DbDataReader materializer using object arrays                    </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1192,9 +1188,8 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1231,12 +1226,12 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>89.16</c:v>
+                  <c:v>66.97</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -1336,9 +1331,8 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1375,12 +1369,12 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>92.24</c:v>
+                  <c:v>70.790000000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000007-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -1480,9 +1474,8 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1519,12 +1512,12 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>96.58</c:v>
+                  <c:v>72.900000000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000008-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -1624,9 +1617,8 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1663,12 +1655,12 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>98.47</c:v>
+                  <c:v>76.17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000009-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -1768,9 +1760,8 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1807,12 +1798,12 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>99.33</c:v>
+                  <c:v>76.47</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000A-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -1912,9 +1903,8 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1951,12 +1941,12 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>103.92</c:v>
+                  <c:v>83.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000B-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -1971,7 +1961,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Entity Framework Core v3.1.8.0 (v3.100.820.42012)                    </c:v>
+                  <c:v>Entity Framework Core v5.0.0.0 (v5.0.20.52303)                       </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2059,9 +2049,8 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2098,12 +2087,12 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>107.93</c:v>
+                  <c:v>84.44</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000C-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -2118,7 +2107,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>NPoco v4.0.2.0 (v4.0.2.0)                                            </c:v>
+                  <c:v>Handcoded materializer using DbDataReader and GetFieldValue&lt;T&gt;       </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2206,9 +2195,8 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2245,12 +2233,12 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>116.19</c:v>
+                  <c:v>89.39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000D-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -2265,7 +2253,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Handcoded materializer using DbDataReader and GetFieldValue&lt;T&gt;       </c:v>
+                  <c:v>NPoco v4.0.3.0 (v4.0.3.0)                                            </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2353,9 +2341,8 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2392,12 +2379,12 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>116.63</c:v>
+                  <c:v>95.03</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000E-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -2500,9 +2487,8 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2539,12 +2525,12 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>118.72</c:v>
+                  <c:v>96.45</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000F-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -2647,9 +2633,8 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2686,12 +2671,12 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>165.75</c:v>
+                  <c:v>134.43</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000010-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -2794,9 +2779,8 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2833,12 +2817,12 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>190.85</c:v>
+                  <c:v>151.31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000011-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -2935,7 +2919,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -2975,7 +2959,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000012-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -3189,7 +3173,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3228,7 +3212,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3297,25 +3280,25 @@
               <c:strCache>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
+                  <c:v>RepoDB (Raw-SQL) v1.12.4.0                                           </c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Handcoded materializer using DbDataReader                            </c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>RepoDB (Raw-SQL) v1.12.0.5                                           </c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>RepoDB (POCO) v1.12.0.5                                              </c:v>
+                  <c:v>RepoDB (POCO) v1.12.4.0                                              </c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>LINQ to DB v3.1.3.0 (v3.1.3) (normal)                                </c:v>
+                  <c:v>LINQ to DB v3.1.6.0 (v3.1.6) (normal)                                </c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>LLBLGen Pro v5.7.0.0 (v5.7.1), Poco with Raw SQL                     </c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>Handcoded materializer using DbDataReader (GetValues(array), boxing) </c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>Raw DbDataReader materializer using object arrays                    </c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Handcoded materializer using DbDataReader (GetValues(array), boxing) </c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Tortuga Chain, Compiled v3.3.2.0                                     </c:v>
@@ -3333,13 +3316,13 @@
                   <c:v>Dapper v2.0.0.0                                                      </c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Entity Framework Core v3.1.8.0 (v3.100.820.42012)                    </c:v>
+                  <c:v>Entity Framework Core v5.0.0.0 (v5.0.20.52303)                       </c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>NPoco v4.0.2.0 (v4.0.2.0)                                            </c:v>
+                  <c:v>Handcoded materializer using DbDataReader and GetFieldValue&lt;T&gt;       </c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>Handcoded materializer using DbDataReader and GetFieldValue&lt;T&gt;       </c:v>
+                  <c:v>NPoco v4.0.3.0 (v4.0.3.0)                                            </c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>ServiceStack OrmLite v5.0.0.0 (v5.0.0.0)                             </c:v>
@@ -3360,63 +3343,63 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>77.36</c:v>
+                  <c:v>59.86</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>77.77</c:v>
+                  <c:v>60.55</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>79.540000000000006</c:v>
+                  <c:v>62.52</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>83.02</c:v>
+                  <c:v>65.02</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>86.39</c:v>
+                  <c:v>66.84</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>87.54</c:v>
+                  <c:v>66.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>89.16</c:v>
+                  <c:v>66.97</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>92.24</c:v>
+                  <c:v>70.790000000000006</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>96.58</c:v>
+                  <c:v>72.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>98.47</c:v>
+                  <c:v>76.17</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>99.33</c:v>
+                  <c:v>76.47</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>103.92</c:v>
+                  <c:v>83.3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>107.93</c:v>
+                  <c:v>84.44</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>116.19</c:v>
+                  <c:v>89.39</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>116.63</c:v>
+                  <c:v>95.03</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>118.72</c:v>
+                  <c:v>96.45</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>165.75</c:v>
+                  <c:v>134.43</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>190.85</c:v>
+                  <c:v>151.31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8BAC-48B0-8D94-A3CB19B3312A}"/>
             </c:ext>
@@ -3454,25 +3437,25 @@
               <c:strCache>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
+                  <c:v>RepoDB (Raw-SQL) v1.12.4.0                                           </c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Handcoded materializer using DbDataReader                            </c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>RepoDB (Raw-SQL) v1.12.0.5                                           </c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>RepoDB (POCO) v1.12.0.5                                              </c:v>
+                  <c:v>RepoDB (POCO) v1.12.4.0                                              </c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>LINQ to DB v3.1.3.0 (v3.1.3) (normal)                                </c:v>
+                  <c:v>LINQ to DB v3.1.6.0 (v3.1.6) (normal)                                </c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>LLBLGen Pro v5.7.0.0 (v5.7.1), Poco with Raw SQL                     </c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>Handcoded materializer using DbDataReader (GetValues(array), boxing) </c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>Raw DbDataReader materializer using object arrays                    </c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Handcoded materializer using DbDataReader (GetValues(array), boxing) </c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Tortuga Chain, Compiled v3.3.2.0                                     </c:v>
@@ -3490,13 +3473,13 @@
                   <c:v>Dapper v2.0.0.0                                                      </c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Entity Framework Core v3.1.8.0 (v3.100.820.42012)                    </c:v>
+                  <c:v>Entity Framework Core v5.0.0.0 (v5.0.20.52303)                       </c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>NPoco v4.0.2.0 (v4.0.2.0)                                            </c:v>
+                  <c:v>Handcoded materializer using DbDataReader and GetFieldValue&lt;T&gt;       </c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>Handcoded materializer using DbDataReader and GetFieldValue&lt;T&gt;       </c:v>
+                  <c:v>NPoco v4.0.3.0 (v4.0.3.0)                                            </c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>ServiceStack OrmLite v5.0.0.0 (v5.0.0.0)                             </c:v>
@@ -3517,63 +3500,63 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>11.5830078125</c:v>
+                  <c:v>11.9609375</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.5830078125</c:v>
+                  <c:v>11.9580078125</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.583984375</c:v>
+                  <c:v>11.9619140625</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.0673828125</c:v>
+                  <c:v>12.44140625</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.5869140625</c:v>
+                  <c:v>11.9619140625</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26.0029296875</c:v>
+                  <c:v>26.5029296875</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26.1279296875</c:v>
+                  <c:v>26.7119140625</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13.5185546875</c:v>
+                  <c:v>13.892578125</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>27.130859375</c:v>
+                  <c:v>27.505859375</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>27.3515625</c:v>
+                  <c:v>28.099609375</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>26.1279296875</c:v>
+                  <c:v>26.5029296875</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>26.1279296875</c:v>
+                  <c:v>26.5029296875</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>26.5068359375</c:v>
+                  <c:v>26.8896484375</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>36.0849609375</c:v>
+                  <c:v>16.66015625</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>16.28515625</c:v>
+                  <c:v>36.462890625</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>29.009765625</c:v>
+                  <c:v>29.384765625</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>42.6591796875</c:v>
+                  <c:v>51.41015625</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>38.681640625</c:v>
+                  <c:v>39.0556640625</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-8BAC-48B0-8D94-A3CB19B3312A}"/>
             </c:ext>
@@ -3709,7 +3692,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3741,14 +3723,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+    <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -4877,7 +4859,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{80B15F94-74E1-4AF2-8970-EB6B8F25ABC1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80B15F94-74E1-4AF2-8970-EB6B8F25ABC1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4913,7 +4895,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9445A904-257A-4875-B69D-7F45EAF9FAEF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9445A904-257A-4875-B69D-7F45EAF9FAEF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5230,584 +5212,602 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BQ21" sqref="BQ21"/>
+    <sheetView tabSelected="1" topLeftCell="Q4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.77734375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="3.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="60.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="60.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.71875" customWidth="1"/>
+    <col min="8" max="8" width="5.6640625" customWidth="1"/>
     <col min="9" max="9" width="6.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="F2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3">
-        <v>103.92</v>
+        <v>83.3</v>
       </c>
       <c r="F3" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="G3">
-        <v>77.36</v>
+        <v>59.86</v>
       </c>
       <c r="H3" s="2">
         <f>I3/1024</f>
-        <v>11.5830078125</v>
+        <v>11.9609375</v>
       </c>
       <c r="I3" s="1">
-        <v>11861</v>
+        <v>12248</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>20</v>
       </c>
       <c r="C4">
-        <v>107.93</v>
+        <v>84.44</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>77.77</v>
+        <v>60.55</v>
       </c>
       <c r="H4" s="2">
         <f>I4/1024</f>
-        <v>11.5830078125</v>
+        <v>11.9580078125</v>
       </c>
       <c r="I4" s="1">
-        <v>11861</v>
+        <v>12245</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>0</v>
       </c>
       <c r="C5">
-        <v>77.36</v>
+        <v>60.55</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G5">
-        <v>79.540000000000006</v>
+        <v>62.52</v>
       </c>
       <c r="H5" s="2">
         <f>I5/1024</f>
-        <v>11.583984375</v>
+        <v>11.9619140625</v>
       </c>
       <c r="I5" s="1">
-        <v>11862</v>
+        <v>12249</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="C6">
-        <v>99.33</v>
+        <v>76.47</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G6">
-        <v>83.02</v>
+        <v>65.02</v>
       </c>
       <c r="H6" s="2">
         <f>I6/1024</f>
-        <v>12.0673828125</v>
+        <v>12.44140625</v>
       </c>
       <c r="I6" s="1">
-        <v>12357</v>
+        <v>12740</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>1</v>
       </c>
       <c r="C7">
-        <v>89.16</v>
+        <v>66.900000000000006</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G7">
-        <v>86.39</v>
+        <v>66.84</v>
       </c>
       <c r="H7" s="2">
         <f>I7/1024</f>
-        <v>11.5869140625</v>
+        <v>11.9619140625</v>
       </c>
       <c r="I7" s="1">
-        <v>11865</v>
+        <v>12249</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8">
-        <v>116.63</v>
+        <v>89.39</v>
       </c>
       <c r="F8" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G8">
-        <v>87.54</v>
+        <v>66.900000000000006</v>
       </c>
       <c r="H8" s="2">
         <f>I8/1024</f>
-        <v>26.0029296875</v>
+        <v>26.5029296875</v>
       </c>
       <c r="I8" s="1">
-        <v>26627</v>
+        <v>27139</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C9">
-        <v>83.02</v>
+        <v>65.02</v>
       </c>
       <c r="F9" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G9">
-        <v>89.16</v>
+        <v>66.97</v>
       </c>
       <c r="H9" s="2">
         <f>I9/1024</f>
-        <v>26.1279296875</v>
+        <v>26.7119140625</v>
       </c>
       <c r="I9" s="1">
-        <v>26755</v>
+        <v>27353</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C10">
-        <v>165.75</v>
+        <v>134.43</v>
       </c>
       <c r="F10" t="s">
         <v>2</v>
       </c>
       <c r="G10">
-        <v>92.24</v>
+        <v>70.790000000000006</v>
       </c>
       <c r="H10" s="2">
         <f>I10/1024</f>
-        <v>13.5185546875</v>
+        <v>13.892578125</v>
       </c>
       <c r="I10" s="1">
-        <v>13843</v>
+        <v>14226</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C11">
-        <v>98.47</v>
+        <v>76.17</v>
       </c>
       <c r="F11" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G11">
-        <v>96.58</v>
+        <v>72.900000000000006</v>
       </c>
       <c r="H11" s="2">
         <f>I11/1024</f>
-        <v>27.130859375</v>
+        <v>27.505859375</v>
       </c>
       <c r="I11" s="1">
-        <v>27782</v>
+        <v>28166</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C12">
-        <v>96.58</v>
+        <v>72.900000000000006</v>
       </c>
       <c r="F12" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G12">
-        <v>98.47</v>
+        <v>76.17</v>
       </c>
       <c r="H12" s="2">
         <f>I12/1024</f>
-        <v>27.3515625</v>
+        <v>28.099609375</v>
       </c>
       <c r="I12" s="1">
-        <v>28008</v>
+        <v>28774</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C13">
-        <v>86.39</v>
+        <v>66.84</v>
       </c>
       <c r="F13" t="s">
         <v>4</v>
       </c>
       <c r="G13">
-        <v>99.33</v>
+        <v>76.47</v>
       </c>
       <c r="H13" s="2">
         <f>I13/1024</f>
-        <v>26.1279296875</v>
+        <v>26.5029296875</v>
       </c>
       <c r="I13" s="1">
-        <v>26755</v>
+        <v>27139</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C14">
-        <v>116.19</v>
+        <v>95.03</v>
       </c>
       <c r="F14" t="s">
         <v>5</v>
       </c>
       <c r="G14">
-        <v>103.92</v>
+        <v>83.3</v>
       </c>
       <c r="H14" s="2">
         <f>I14/1024</f>
-        <v>26.1279296875</v>
+        <v>26.5029296875</v>
       </c>
       <c r="I14" s="1">
-        <v>26755</v>
+        <v>27139</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>3</v>
       </c>
       <c r="C15">
-        <v>87.54</v>
+        <v>66.97</v>
       </c>
       <c r="F15" t="s">
         <v>20</v>
       </c>
       <c r="G15">
-        <v>107.93</v>
+        <v>84.44</v>
       </c>
       <c r="H15" s="2">
         <f>I15/1024</f>
-        <v>26.5068359375</v>
+        <v>26.8896484375</v>
       </c>
       <c r="I15" s="1">
-        <v>27143</v>
+        <v>27535</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C16">
-        <v>79.540000000000006</v>
+        <v>62.52</v>
       </c>
       <c r="F16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G16">
-        <v>116.19</v>
+        <v>89.39</v>
       </c>
       <c r="H16" s="2">
         <f>I16/1024</f>
-        <v>36.0849609375</v>
+        <v>16.66015625</v>
       </c>
       <c r="I16" s="1">
-        <v>36951</v>
+        <v>17060</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C17">
-        <v>77.77</v>
+        <v>59.86</v>
       </c>
       <c r="F17" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="G17">
-        <v>116.63</v>
+        <v>95.03</v>
       </c>
       <c r="H17" s="2">
         <f>I17/1024</f>
-        <v>16.28515625</v>
+        <v>36.462890625</v>
       </c>
       <c r="I17" s="1">
-        <v>16676</v>
+        <v>37338</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>7</v>
       </c>
       <c r="C18">
-        <v>118.72</v>
+        <v>96.45</v>
       </c>
       <c r="F18" t="s">
         <v>7</v>
       </c>
       <c r="G18">
-        <v>118.72</v>
+        <v>96.45</v>
       </c>
       <c r="H18" s="2">
         <f>I18/1024</f>
-        <v>29.009765625</v>
+        <v>29.384765625</v>
       </c>
       <c r="I18" s="1">
-        <v>29706</v>
+        <v>30090</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C19">
-        <v>190.85</v>
+        <v>151.31</v>
       </c>
       <c r="F19" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="G19">
-        <v>165.75</v>
+        <v>134.43</v>
       </c>
       <c r="H19" s="2">
         <f>I19/1024</f>
-        <v>42.6591796875</v>
+        <v>51.41015625</v>
       </c>
       <c r="I19" s="1">
-        <v>43683</v>
+        <v>52644</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>2</v>
       </c>
       <c r="C20">
-        <v>92.24</v>
+        <v>70.790000000000006</v>
       </c>
       <c r="F20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G20">
-        <v>190.85</v>
+        <v>151.31</v>
       </c>
       <c r="H20" s="2">
         <f>I20/1024</f>
-        <v>38.681640625</v>
+        <v>39.0556640625</v>
       </c>
       <c r="I20" s="1">
-        <v>39610</v>
+        <v>39993</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>5</v>
       </c>
       <c r="C24" s="1">
-        <v>26755</v>
+        <v>27139</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>20</v>
       </c>
       <c r="C25" s="1">
-        <v>27143</v>
+        <v>27535</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>0</v>
       </c>
       <c r="C26" s="1">
-        <v>11861</v>
+        <v>12245</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>4</v>
       </c>
       <c r="C27" s="1">
-        <v>26755</v>
+        <v>27139</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>1</v>
       </c>
       <c r="C28" s="1">
-        <v>26755</v>
+        <v>27139</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>6</v>
       </c>
       <c r="C29" s="1">
-        <v>16676</v>
+        <v>17060</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="1">
+        <v>12740</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="1">
-        <v>12357</v>
+      <c r="C31" s="1">
+        <v>52644</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B31" t="s">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="1">
+        <v>28774</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="1">
+        <v>28166</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="1">
+        <v>12249</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="1">
-        <v>43683</v>
+      <c r="C35" s="1">
+        <v>37338</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B32" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" s="1">
-        <v>28008</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B33" t="s">
-        <v>18</v>
-      </c>
-      <c r="C33" s="1">
-        <v>27782</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B34" t="s">
-        <v>17</v>
-      </c>
-      <c r="C34" s="1">
-        <v>11865</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B35" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="1">
-        <v>36951</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>3</v>
       </c>
       <c r="C36" s="1">
-        <v>26627</v>
+        <v>27353</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C37" s="1">
-        <v>11862</v>
+        <v>12249</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C38" s="1">
-        <v>11861</v>
+        <v>12248</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>7</v>
       </c>
       <c r="C39" s="1">
-        <v>29706</v>
+        <v>30090</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C40" s="1">
-        <v>39610</v>
+        <v>39993</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>2</v>
       </c>
       <c r="C41" s="1">
-        <v>13843</v>
+        <v>14226</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="F3:I20">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F3:I20">
     <sortCondition ref="G3:G20"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;1#&amp;"Arial Black"&amp;10&amp;K4099DAINTERNAL</oddFooter>
+  </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003DB59D54AAC4B24EA9A98B6159AEDD81" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a776c128c0314cb3d9aae2760f8fd3ed">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a97ded03-527c-4a0c-b158-f2940a76ab81" xmlns:ns4="a35486a1-8de9-475b-b6e0-d65b6b15b04d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a509177177e4963985278f96f91598b3" ns3:_="" ns4:_="">
     <xsd:import namespace="a97ded03-527c-4a0c-b158-f2940a76ab81"/>
@@ -6030,36 +6030,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32778BE5-BD41-4D93-AA7F-37C8F944F48B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6DAE986B-EB8C-45F5-81CA-F200183CDC61}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a97ded03-527c-4a0c-b158-f2940a76ab81"/>
-    <ds:schemaRef ds:uri="a35486a1-8de9-475b-b6e0-d65b6b15b04d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6082,9 +6056,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6DAE986B-EB8C-45F5-81CA-F200183CDC61}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32778BE5-BD41-4D93-AA7F-37C8F944F48B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a97ded03-527c-4a0c-b158-f2940a76ab81"/>
+    <ds:schemaRef ds:uri="a35486a1-8de9-475b-b6e0-d65b6b15b04d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
More updates on the colorings.
</commit_message>
<xml_diff>
--- a/assets/ORM Statistics Official Result.xlsx
+++ b/assets/ORM Statistics Official Result.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\GitHub\RepoDB.NET\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MichaelP\Source\Repos\GitHub\RepoDb.NET\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295B7EF3-FD85-45D3-9CB0-1974DAE94112}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="53892" yWindow="-108" windowWidth="25416" windowHeight="15516" tabRatio="538" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="53892" yWindow="-108" windowWidth="25416" windowHeight="15516" tabRatio="538"/>
   </bookViews>
   <sheets>
     <sheet name="Entries" sheetId="1" r:id="rId1"/>
@@ -104,7 +103,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -153,6 +152,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF1A9643"/>
+      <color rgb="FF247422"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -165,7 +170,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -218,6 +223,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -345,8 +351,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -388,7 +395,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -485,8 +492,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -528,7 +536,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -625,8 +633,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -668,7 +677,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -765,8 +774,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -808,7 +818,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -905,8 +915,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -948,7 +959,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -1045,8 +1056,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1088,7 +1100,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -1188,8 +1200,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1231,7 +1244,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -1331,8 +1344,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1374,7 +1388,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000007-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -1474,8 +1488,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1517,7 +1532,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000008-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -1617,8 +1632,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1660,7 +1676,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000009-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -1760,8 +1776,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1803,7 +1820,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000A-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -1903,8 +1920,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1946,7 +1964,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000B-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -2049,8 +2067,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2092,7 +2111,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000C-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -2195,8 +2214,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2238,7 +2258,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000D-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -2341,8 +2361,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2384,7 +2405,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000E-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -2487,8 +2508,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2530,7 +2552,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000F-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -2633,8 +2655,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2676,7 +2699,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000010-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -2779,8 +2802,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2822,7 +2846,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000011-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -2919,7 +2943,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -2959,7 +2983,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000012-80C2-4885-9FE9-DD723A60ADE7}"/>
             </c:ext>
@@ -2976,11 +3000,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="1087893440"/>
-        <c:axId val="1087893984"/>
+        <c:axId val="-473562704"/>
+        <c:axId val="-473582832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1087893440"/>
+        <c:axId val="-473562704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3023,7 +3047,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1087893984"/>
+        <c:crossAx val="-473582832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3031,7 +3055,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1087893984"/>
+        <c:axId val="-473582832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3082,7 +3106,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1087893440"/>
+        <c:crossAx val="-473562704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3173,7 +3197,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3193,25 +3217,26 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mj-lt"/>
+                <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mj-ea"/>
-                <a:cs typeface="+mj-cs"/>
+                <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" b="1"/>
               <a:t>ORM Statistics Official Result</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3225,16 +3250,16 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mj-lt"/>
+              <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mj-ea"/>
-              <a:cs typeface="+mj-cs"/>
+              <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -3264,14 +3289,18 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:alpha val="70000"/>
-              </a:schemeClr>
+              <a:srgbClr val="1A9643"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                <a:prstClr val="black">
+                  <a:alpha val="40000"/>
+                </a:prstClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -3399,7 +3428,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8BAC-48B0-8D94-A3CB19B3312A}"/>
             </c:ext>
@@ -3421,14 +3450,20 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2">
+              <a:srgbClr val="FFC000">
                 <a:alpha val="70000"/>
-              </a:schemeClr>
+              </a:srgbClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                <a:prstClr val="black">
+                  <a:alpha val="40000"/>
+                </a:prstClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -3556,7 +3591,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-8BAC-48B0-8D94-A3CB19B3312A}"/>
             </c:ext>
@@ -3571,12 +3606,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="80"/>
-        <c:overlap val="25"/>
-        <c:axId val="1087901600"/>
-        <c:axId val="1087883648"/>
+        <c:axId val="-473562160"/>
+        <c:axId val="-473576304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1087901600"/>
+        <c:axId val="-473562160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3604,22 +3638,22 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" normalizeH="0" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1087883648"/>
+        <c:crossAx val="-473576304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3627,7 +3661,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1087883648"/>
+        <c:axId val="-473576304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3670,15 +3704,15 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1087901600"/>
+        <c:crossAx val="-473562160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3692,6 +3726,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3712,9 +3747,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -3723,14 +3758,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3752,7 +3787,10 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -4859,7 +4897,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80B15F94-74E1-4AF2-8970-EB6B8F25ABC1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{80B15F94-74E1-4AF2-8970-EB6B8F25ABC1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4882,20 +4920,20 @@
       <xdr:col>28</xdr:col>
       <xdr:colOff>45720</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
+      <xdr:rowOff>76198</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>79</xdr:col>
-      <xdr:colOff>49306</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>134471</xdr:rowOff>
+      <xdr:col>93</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9445A904-257A-4875-B69D-7F45EAF9FAEF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9445A904-257A-4875-B69D-7F45EAF9FAEF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5212,14 +5250,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CB14" sqref="CB14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="3.77734375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="60.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
@@ -5229,7 +5267,7 @@
     <col min="9" max="9" width="6.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
@@ -5249,7 +5287,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -5263,14 +5301,14 @@
         <v>59.86</v>
       </c>
       <c r="H3" s="2">
-        <f>I3/1024</f>
+        <f t="shared" ref="H3:H20" si="0">I3/1024</f>
         <v>11.9609375</v>
       </c>
       <c r="I3" s="1">
         <v>12248</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
         <v>20</v>
       </c>
@@ -5284,14 +5322,14 @@
         <v>60.55</v>
       </c>
       <c r="H4" s="2">
-        <f>I4/1024</f>
+        <f t="shared" si="0"/>
         <v>11.9580078125</v>
       </c>
       <c r="I4" s="1">
         <v>12245</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
         <v>0</v>
       </c>
@@ -5305,14 +5343,14 @@
         <v>62.52</v>
       </c>
       <c r="H5" s="2">
-        <f>I5/1024</f>
+        <f t="shared" si="0"/>
         <v>11.9619140625</v>
       </c>
       <c r="I5" s="1">
         <v>12249</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -5326,14 +5364,14 @@
         <v>65.02</v>
       </c>
       <c r="H6" s="2">
-        <f>I6/1024</f>
+        <f t="shared" si="0"/>
         <v>12.44140625</v>
       </c>
       <c r="I6" s="1">
         <v>12740</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
         <v>1</v>
       </c>
@@ -5347,14 +5385,14 @@
         <v>66.84</v>
       </c>
       <c r="H7" s="2">
-        <f>I7/1024</f>
+        <f t="shared" si="0"/>
         <v>11.9619140625</v>
       </c>
       <c r="I7" s="1">
         <v>12249</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -5368,14 +5406,14 @@
         <v>66.900000000000006</v>
       </c>
       <c r="H8" s="2">
-        <f>I8/1024</f>
+        <f t="shared" si="0"/>
         <v>26.5029296875</v>
       </c>
       <c r="I8" s="1">
         <v>27139</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
         <v>19</v>
       </c>
@@ -5389,14 +5427,14 @@
         <v>66.97</v>
       </c>
       <c r="H9" s="2">
-        <f>I9/1024</f>
+        <f t="shared" si="0"/>
         <v>26.7119140625</v>
       </c>
       <c r="I9" s="1">
         <v>27353</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
         <v>16</v>
       </c>
@@ -5410,14 +5448,14 @@
         <v>70.790000000000006</v>
       </c>
       <c r="H10" s="2">
-        <f>I10/1024</f>
+        <f t="shared" si="0"/>
         <v>13.892578125</v>
       </c>
       <c r="I10" s="1">
         <v>14226</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
         <v>15</v>
       </c>
@@ -5431,14 +5469,14 @@
         <v>72.900000000000006</v>
       </c>
       <c r="H11" s="2">
-        <f>I11/1024</f>
+        <f t="shared" si="0"/>
         <v>27.505859375</v>
       </c>
       <c r="I11" s="1">
         <v>28166</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
         <v>14</v>
       </c>
@@ -5452,14 +5490,14 @@
         <v>76.17</v>
       </c>
       <c r="H12" s="2">
-        <f>I12/1024</f>
+        <f t="shared" si="0"/>
         <v>28.099609375</v>
       </c>
       <c r="I12" s="1">
         <v>28774</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B13" t="s">
         <v>13</v>
       </c>
@@ -5473,14 +5511,14 @@
         <v>76.47</v>
       </c>
       <c r="H13" s="2">
-        <f>I13/1024</f>
+        <f t="shared" si="0"/>
         <v>26.5029296875</v>
       </c>
       <c r="I13" s="1">
         <v>27139</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
         <v>21</v>
       </c>
@@ -5494,14 +5532,14 @@
         <v>83.3</v>
       </c>
       <c r="H14" s="2">
-        <f>I14/1024</f>
+        <f t="shared" si="0"/>
         <v>26.5029296875</v>
       </c>
       <c r="I14" s="1">
         <v>27139</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
         <v>3</v>
       </c>
@@ -5515,14 +5553,14 @@
         <v>84.44</v>
       </c>
       <c r="H15" s="2">
-        <f>I15/1024</f>
+        <f t="shared" si="0"/>
         <v>26.8896484375</v>
       </c>
       <c r="I15" s="1">
         <v>27535</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
         <v>18</v>
       </c>
@@ -5536,14 +5574,14 @@
         <v>89.39</v>
       </c>
       <c r="H16" s="2">
-        <f>I16/1024</f>
+        <f t="shared" si="0"/>
         <v>16.66015625</v>
       </c>
       <c r="I16" s="1">
         <v>17060</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B17" t="s">
         <v>17</v>
       </c>
@@ -5557,14 +5595,14 @@
         <v>95.03</v>
       </c>
       <c r="H17" s="2">
-        <f>I17/1024</f>
+        <f t="shared" si="0"/>
         <v>36.462890625</v>
       </c>
       <c r="I17" s="1">
         <v>37338</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B18" t="s">
         <v>7</v>
       </c>
@@ -5578,14 +5616,14 @@
         <v>96.45</v>
       </c>
       <c r="H18" s="2">
-        <f>I18/1024</f>
+        <f t="shared" si="0"/>
         <v>29.384765625</v>
       </c>
       <c r="I18" s="1">
         <v>30090</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B19" t="s">
         <v>8</v>
       </c>
@@ -5599,14 +5637,14 @@
         <v>134.43</v>
       </c>
       <c r="H19" s="2">
-        <f>I19/1024</f>
+        <f t="shared" si="0"/>
         <v>51.41015625</v>
       </c>
       <c r="I19" s="1">
         <v>52644</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B20" t="s">
         <v>2</v>
       </c>
@@ -5620,14 +5658,14 @@
         <v>151.31</v>
       </c>
       <c r="H20" s="2">
-        <f>I20/1024</f>
+        <f t="shared" si="0"/>
         <v>39.0556640625</v>
       </c>
       <c r="I20" s="1">
         <v>39993</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B23" s="3" t="s">
         <v>9</v>
       </c>
@@ -5635,7 +5673,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
         <v>5</v>
       </c>
@@ -5643,7 +5681,7 @@
         <v>27139</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B25" t="s">
         <v>20</v>
       </c>
@@ -5651,7 +5689,7 @@
         <v>27535</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B26" t="s">
         <v>0</v>
       </c>
@@ -5659,7 +5697,7 @@
         <v>12245</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B27" t="s">
         <v>4</v>
       </c>
@@ -5667,7 +5705,7 @@
         <v>27139</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B28" t="s">
         <v>1</v>
       </c>
@@ -5675,7 +5713,7 @@
         <v>27139</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
         <v>6</v>
       </c>
@@ -5683,7 +5721,7 @@
         <v>17060</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B30" t="s">
         <v>19</v>
       </c>
@@ -5691,7 +5729,7 @@
         <v>12740</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B31" t="s">
         <v>16</v>
       </c>
@@ -5699,7 +5737,7 @@
         <v>52644</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B32" t="s">
         <v>15</v>
       </c>
@@ -5707,7 +5745,7 @@
         <v>28774</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B33" t="s">
         <v>14</v>
       </c>
@@ -5715,7 +5753,7 @@
         <v>28166</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B34" t="s">
         <v>13</v>
       </c>
@@ -5723,7 +5761,7 @@
         <v>12249</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B35" t="s">
         <v>21</v>
       </c>
@@ -5731,7 +5769,7 @@
         <v>37338</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B36" t="s">
         <v>3</v>
       </c>
@@ -5739,7 +5777,7 @@
         <v>27353</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B37" t="s">
         <v>18</v>
       </c>
@@ -5747,7 +5785,7 @@
         <v>12249</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B38" t="s">
         <v>17</v>
       </c>
@@ -5755,7 +5793,7 @@
         <v>12248</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B39" t="s">
         <v>7</v>
       </c>
@@ -5763,7 +5801,7 @@
         <v>30090</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B40" t="s">
         <v>8</v>
       </c>
@@ -5771,7 +5809,7 @@
         <v>39993</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B41" t="s">
         <v>2</v>
       </c>
@@ -5780,7 +5818,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F3:I20">
+  <sortState ref="F3:I20">
     <sortCondition ref="G3:G20"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5802,12 +5840,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003DB59D54AAC4B24EA9A98B6159AEDD81" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a776c128c0314cb3d9aae2760f8fd3ed">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a97ded03-527c-4a0c-b158-f2940a76ab81" xmlns:ns4="a35486a1-8de9-475b-b6e0-d65b6b15b04d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a509177177e4963985278f96f91598b3" ns3:_="" ns4:_="">
     <xsd:import namespace="a97ded03-527c-4a0c-b158-f2940a76ab81"/>
@@ -6030,6 +6062,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6DAE986B-EB8C-45F5-81CA-F200183CDC61}">
   <ds:schemaRefs>
@@ -6039,23 +6077,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1357F301-0B8B-4188-9FBA-2D28B749906F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="a35486a1-8de9-475b-b6e0-d65b6b15b04d"/>
-    <ds:schemaRef ds:uri="a97ded03-527c-4a0c-b158-f2940a76ab81"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32778BE5-BD41-4D93-AA7F-37C8F944F48B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6072,4 +6093,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1357F301-0B8B-4188-9FBA-2D28B749906F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="a35486a1-8de9-475b-b6e0-d65b6b15b04d"/>
+    <ds:schemaRef ds:uri="a97ded03-527c-4a0c-b158-f2940a76ab81"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>